<commit_message>
Added Functionality for r/animenews
</commit_message>
<xml_diff>
--- a/anime_news.xlsx
+++ b/anime_news.xlsx
@@ -7,13 +7,14 @@
     <sheet sheetId="1" name="MyAnimeList News" state="visible" r:id="rId4"/>
     <sheet sheetId="2" name="Anime News Network News" state="visible" r:id="rId5"/>
     <sheet sheetId="3" name="Anime Megathread Top Comments" state="visible" r:id="rId6"/>
+    <sheet sheetId="4" name="AnimeNews Subreddit" state="visible" r:id="rId7"/>
   </sheets>
   <calcPr calcId="171027"/>
 </workbook>
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="417" uniqueCount="412">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="573" uniqueCount="510">
   <si>
     <t>Title</t>
   </si>
@@ -24,6 +25,42 @@
     <t>Content</t>
   </si>
   <si>
+    <t>Cygames Announces 'Yuuki Bakuhatsu Bang Bravern' Original TV Anime</t>
+  </si>
+  <si>
+    <t>https://myanimelist.net/news/69291235</t>
+  </si>
+  <si>
+    <t>Cygames announced an original television anime titled Yuuki Bakuhatsu Bang Bravern (Bang Brave Bang Bravern) on Monday. The video game developer also opened an official website, revealing the lead staff, a teaser promo, and teaser visual (pictured). Masami Oobari (Prism Ark, Bubb...</t>
+  </si>
+  <si>
+    <t>'Girls Band Cry' Reveals Main Cast, Staff, Key Visual</t>
+  </si>
+  <si>
+    <t>https://myanimelist.net/news/69290954</t>
+  </si>
+  <si>
+    <t>The official website of Toei Animation's Girls Band Cry original anime revealed the cast, staff, key visual (pictured), and two music videos by the Togenashi Togeari unit on Monday. Staff Original Work, Planning, Production: Toei Animation Director: Kazuo Sakai (Love Live! Sunshi...</t>
+  </si>
+  <si>
+    <t>'Kage no Jitsuryokusha ni Naritakute!' 2nd Season Reveals Additional Cast, Second Promo, Fall 2023 Premiere</t>
+  </si>
+  <si>
+    <t>https://myanimelist.net/news/69284569</t>
+  </si>
+  <si>
+    <t>The official website of the television anime adaptation of Daisuke Aizawa's Kage no Jitsuryokusha ni Naritakute! (The Eminence in Shadow) light novel revealed on Sunday additional cast and a second promotional video for the second season. The new season is scheduled to premiere i...</t>
+  </si>
+  <si>
+    <t>'Bleach: Sennen Kessen-hen - Ketsubetsu-tan' Reveals Additional Cast, Opening Theme, First Promo</t>
+  </si>
+  <si>
+    <t>https://myanimelist.net/news/69283316</t>
+  </si>
+  <si>
+    <t>The official website of the Bleach: Sennen Kessen-hen (Bleach: Thousand-Year Blood War) television anime revealed on Sunday four additional cast, opening theme, key visual (pictured), and a promotional video for the second cour. Ketsubetsu-tan is scheduled to premiere on July 8 a...</t>
+  </si>
+  <si>
     <t>'BanG Dream! It's MyGO!!!!!' Reveals Additional Staff, Ending Theme</t>
   </si>
   <si>
@@ -168,40 +205,283 @@
     <t>The Kessoku Band Live: Kousei event announced a compilation movie for the Bocchi the Rock! anime series on Sunday, revealing a key visual (pictured) and an announcement promo. The movie will open in theaters in Japan in Spring 2024. The television anime produced by CloverWorks ai...</t>
   </si>
   <si>
-    <t>'Synduality: Noir' Announces Additional Cast, Ending Theme</t>
-  </si>
-  <si>
-    <t>https://myanimelist.net/news/69240627</t>
-  </si>
-  <si>
-    <t>The official website of the Synduality: Noir television anime revealed three supporting cast members and the ending theme on Sunday. The anime is scheduled to premiere on July 11 at 12:00 a.m. on TV Tokyo, BS-NTV, and other channels. It will also stream worldwide exclusively on D...</t>
-  </si>
-  <si>
-    <t>'Nanatsu no Maken ga Shihai suru' Announces Supporting Cast</t>
-  </si>
-  <si>
-    <t>https://myanimelist.net/news/69229712</t>
-  </si>
-  <si>
-    <t>The official website of the Nanatsu no Maken ga Shihai suru (Reign of the Seven Spellblades) television anime series announced on Friday three additional cast members. The anime is scheduled to premiere in July 2023. Cast Esmeralda: Atsuko Tanaka (JoJo no Kimyou na Bouken (TV))...</t>
-  </si>
-  <si>
-    <t>'Higeki no Genkyou to Naru Saikyou Gedou Last Boss Joou wa Tami no Tame ni Tsukushimasu.' Unveils Additional Cast, Theme Songs</t>
-  </si>
-  <si>
-    <t>https://myanimelist.net/news/69223570</t>
-  </si>
-  <si>
-    <t>The official website of the television anime adaptation of Tenichi's Higeki no Genkyou to Naru Saikyou Gedou Last Boss Joou wa Tami no Tame ni Tsukushimasu. (The Most Heretical Last Boss Queen: From Villainess to Savior) light novel unveiled additional cast members and the theme...</t>
-  </si>
-  <si>
-    <t>Manga 'Medalist' Gets TV Anime</t>
-  </si>
-  <si>
-    <t>https://myanimelist.net/news/69223465</t>
-  </si>
-  <si>
-    <t>Publishing company Kadokawa opened an official website for a television anime adaptation of Tsurumaikada's Medalist manga on Thursday, revealing the main staff and a teaser visual (pictured). Staff Director: Yasutaka Yamamoto (Noblesse, Nekopara) Series Composition: Jukki Hanada...</t>
+    <t>Spider-Man: Across the Spider-Verse Film Gets Manga Spinoff About Doc Ock in Schoolgirl's Body</t>
+  </si>
+  <si>
+    <t>https://www.animenewsnetwork.com/news/2023-05-29/spider-man-across-the-spider-verse-film-gets-manga-spinoff-about-doc-ock-in-schoolgirl-body/.198587</t>
+  </si>
+  <si>
+    <t>My Hero Academia: Vigilantes' Hideyuki Furuhashi, Betten Court draw manga launching on June 20</t>
+  </si>
+  <si>
+    <t>Golden Kamuy Anime Season 4 Casts Kousuke Toriumi</t>
+  </si>
+  <si>
+    <t>https://www.animenewsnetwork.com/news/2023-05-29/golden-kamuy-anime-season-4-casts-kousuke-toriumi/.198586</t>
+  </si>
+  <si>
+    <t>Toriumi plays Takuboku Ishikawa</t>
+  </si>
+  <si>
+    <t>Insomniacs After School Anime Casts Sora Amamiya as Isaki's Big Sister</t>
+  </si>
+  <si>
+    <t>https://www.animenewsnetwork.com/news/2023-05-29/insomniacs-after-school-anime-casts-sora-amamiya-as-isaki-big-sister/.198585</t>
+  </si>
+  <si>
+    <t>Haya Magari appears in next week's episode</t>
+  </si>
+  <si>
+    <t>Mobile Suit Gundam: Hathaway's Flash Manga Ends 1st Part</t>
+  </si>
+  <si>
+    <t>https://www.animenewsnetwork.com/news/2023-05-29/mobile-suit-gundam-hathaway-flash-manga-ends-1st-part/.198541</t>
+  </si>
+  <si>
+    <t>Manga's 1st part ends on June 26</t>
+  </si>
+  <si>
+    <t>Anime Expo Hosts Yoshiki, Takayuki Hirao, Cast of Love Live! Franchise, More</t>
+  </si>
+  <si>
+    <t>https://www.animenewsnetwork.com/news/2023-05-29/anime-expo-hosts-yoshiki-takayuki-hirao-cast-of-love-live-franchise-more/.198539</t>
+  </si>
+  <si>
+    <t>Voice actor Masakazu Morita, Zom 100 manga creator Kotaro Takata also attend event</t>
+  </si>
+  <si>
+    <t>Crimson Hero's Mitsuba Takanashi Goes on Hiatus for Breast Cancer Surgery, Treatment</t>
+  </si>
+  <si>
+    <t>https://www.animenewsnetwork.com/news/2023-05-29/crimson-hero-mitsuba-takanashi-goes-on-hiatus-for-breast-cancer-surgery-treatment/.198562</t>
+  </si>
+  <si>
+    <t>Takanashi's ongoing Otome Tsubaki wa Warawanai manga goes on hiatus indefinitely</t>
+  </si>
+  <si>
+    <t>Bleach: Thousand-Year Blood War Anime's Video Unveils New Opening Song, More Cast, July 8 Return</t>
+  </si>
+  <si>
+    <t>https://www.animenewsnetwork.com/news/2023-05-28/bleach-thousand-year-blood-war-anime-video-unveils-new-opening-song-more-cast-july-8-return/.198543</t>
+  </si>
+  <si>
+    <t>Aoi Yūki, Tsuyoshi Koyama, Sōichiro Hoshi, Nao Tōyama, rock band w.o.d. join anime</t>
+  </si>
+  <si>
+    <t>Demon Slayer: Swordsmith Village Arc Anime Casts Kengo Kawanishi Twice &amp; Manami Numakura</t>
+  </si>
+  <si>
+    <t>https://www.animenewsnetwork.com/news/2023-05-28/demon-slayer-swordsmith-village-arc-anime-casts-kengo-kawanishi-twice-and-manami-numakura/.198549</t>
+  </si>
+  <si>
+    <t>Kawanishi plays dual roles; Kentarō Kumagai, Atsushi Ono also cast</t>
+  </si>
+  <si>
+    <t>Zom 100: Bucket List of the Dead Anime Debuts on Hulu in U.S. on July 9</t>
+  </si>
+  <si>
+    <t>https://www.animenewsnetwork.com/news/2023-05-28/zom-100-bucket-list-of-the-dead-anime-debuts-on-hulu-in-u.s-on-july-9/.198537</t>
+  </si>
+  <si>
+    <t>Viz Media to also stream anime on Netflix, "other streaming platforms"</t>
+  </si>
+  <si>
+    <t>Yumemiru Danshi wa Genjitsushugisha Anime Reveals Opening, Ending Theme Song Artists</t>
+  </si>
+  <si>
+    <t>https://www.animenewsnetwork.com/news/2023-05-29/yumemiru-danshi-wa-genjitsushugisha-anime-reveals-opening-ending-theme-song-artists/.198577</t>
+  </si>
+  <si>
+    <t>Kaori Ishihara performs opening, Akiho Suzumoto performs ending for summer anime</t>
+  </si>
+  <si>
+    <t>Sorcerous Stabber Orphen Anime's Sanctuary Arc Casts Haruka Fushimi</t>
+  </si>
+  <si>
+    <t>https://www.animenewsnetwork.com/news/2023-05-29/sorcerous-stabber-orphen-anime-sanctuary-arc-casts-haruka-fushimi/.198578</t>
+  </si>
+  <si>
+    <t>Fushimi voices Isabella in new series</t>
+  </si>
+  <si>
+    <t>Suzume Film Ends Theatrical Run in Japan with 14.79 Billion Yen Total Box Office Earnings</t>
+  </si>
+  <si>
+    <t>https://www.animenewsnetwork.com/news/2023-05-29/suzume-film-ends-theatrical-run-in-japan-with-14.79-billion-yen-total-box-office-earnings/.198572</t>
+  </si>
+  <si>
+    <t>Film ranked #8 in its 29th, final weekend in theaters</t>
+  </si>
+  <si>
+    <t>The First Slam Dunk Surpasses Weathering With You, Becomes 9th Highest-Earning Anime Film in Japan</t>
+  </si>
+  <si>
+    <t>https://www.animenewsnetwork.com/news/2023-05-29/the-first-slam-dunk-surpasses-weathering-with-you-becomes-9th-highest-earning-anime-film-in-japan/.198573</t>
+  </si>
+  <si>
+    <t>Film is 15th highest-earning film of all time in Japan, below Suzume</t>
+  </si>
+  <si>
+    <t>The Super Mario Bros. Movie Tops 10 Billion Yen in Japan</t>
+  </si>
+  <si>
+    <t>https://www.animenewsnetwork.com/news/2023-05-29/the-super-mario-bros-movie-tops-10-billion-yen-in-japan/.198568</t>
+  </si>
+  <si>
+    <t>Film has earned worldwide total of US$1.27 billion</t>
+  </si>
+  <si>
+    <t>Tekken 8 Fighting Game Reveals Gameplay Trailer for Bryan Fury</t>
+  </si>
+  <si>
+    <t>https://www.animenewsnetwork.com/news/2023-05-29/tekken-8-fighting-game-reveals-gameplay-trailer-for-bryan-fury/.198566</t>
+  </si>
+  <si>
+    <t>Game under development for PS5, Xbox Series X|S, PC</t>
+  </si>
+  <si>
+    <t>The Masterful Cat Is Depressed Again Today Anime Previewed in 2nd Promo Video</t>
+  </si>
+  <si>
+    <t>https://www.animenewsnetwork.com/news/2023-05-29/the-masterful-cat-is-depressed-again-today-anime-previewed-in-2nd-promo-video/.198564</t>
+  </si>
+  <si>
+    <t>somei performs opening theme for series premiering on July 7</t>
+  </si>
+  <si>
+    <t>Gundam Gets The Battle Tales of Flanagan Boon U.C. Spinoff Manga</t>
+  </si>
+  <si>
+    <t>https://www.animenewsnetwork.com/news/2023-05-29/gundam-gets-the-battle-tales-of-flanagan-boon-u.c-spinoff-manga/.198558</t>
+  </si>
+  <si>
+    <t>New manga centers on minor character Flanagan Boon from episode 28 of Mobile Suit Gundam</t>
+  </si>
+  <si>
+    <t>Tatsuwo's Dawn of the Witch Manga Adaptation Ends</t>
+  </si>
+  <si>
+    <t>https://www.animenewsnetwork.com/news/2023-05-29/tatsuwo-dawn-of-the-witch-manga-adaptation-ends/.198540</t>
+  </si>
+  <si>
+    <t>Manga launched in 2019</t>
+  </si>
+  <si>
+    <t>Anime Limited to Release Great Pretender Anime on Home Video in U.S., Canada, U.K., Ireland</t>
+  </si>
+  <si>
+    <t>https://www.animenewsnetwork.com/news/2023-05-29/anime-limited-to-release-great-pretender-anime-on-home-video-in-u.s-canada-u.k-ireland/.198544</t>
+  </si>
+  <si>
+    <t>Company also announces Collector's Edition for anime series</t>
+  </si>
+  <si>
+    <t>Yen Press Reveals New Licenses Including Kana Akatsuki's Award-Winning Agent of the Four Seasons Novel</t>
+  </si>
+  <si>
+    <t>https://www.animenewsnetwork.com/news/2023-05-27/yen-press-reveals-new-licenses-including-kana-akatsuki-award-winning-agent-of-the-four-seasons-novel/.198529</t>
+  </si>
+  <si>
+    <t>Fruits Basket artbook, Higurashi When They Cry: GOU anthology, more licensed</t>
+  </si>
+  <si>
+    <t>Live-Action 'Do It Yourself!!' Series Unveils Cast, July 4 Premiere</t>
+  </si>
+  <si>
+    <t>https://www.animenewsnetwork.com/news/2023-05-28/live-action-do-it-yourself-series-unveils-cast-july-4-premiere/.198542</t>
+  </si>
+  <si>
+    <t>Hinatazaka46 idol Hinano Kamimura plays protagonist Serufu</t>
+  </si>
+  <si>
+    <t>The Fable: The Second Contact Manga Ends in 5 Chapters</t>
+  </si>
+  <si>
+    <t>https://www.animenewsnetwork.com/news/2023-05-28/the-fable-the-second-contact-manga-ends-in-5-chapters/.198534</t>
+  </si>
+  <si>
+    <t>Sequel series about genius hitman launched in July 2021</t>
+  </si>
+  <si>
+    <t>Manga Up! Launches The Red Ranger Becomes an Adventurer in Another World Manga in English, Adds Durarara!! Manga</t>
+  </si>
+  <si>
+    <t>https://www.animenewsnetwork.com/news/2023-05-28/manga-up-launches-the-red-ranger-becomes-an-adventurer-in-another-world-manga-in-english-adds-/.198512</t>
+  </si>
+  <si>
+    <t>The Red Ranger Becomes an Adventurer in Another World manga launched in November 2020</t>
+  </si>
+  <si>
+    <t>Bleach: Thousand-Year Blood War Anime's Part 2 Premieres Overseas on July 8</t>
+  </si>
+  <si>
+    <t>https://www.animenewsnetwork.com/news/2023-05-28/bleach-thousand-year-blood-war-anime-part-2-premieres-overseas-on-july-8/.198548</t>
+  </si>
+  <si>
+    <t>Anime premieres in U.S. on Hulu, Latin America on Star+, in other select countries internationally on Disney+ at 7:30 AM PDT.</t>
+  </si>
+  <si>
+    <t>Aya Shouoto Ends Kagetoki-sama no Kurenai Kōkyū Manga, Launches The Demon Prince of Momochi House Sequel Manga</t>
+  </si>
+  <si>
+    <t>https://www.animenewsnetwork.com/news/2023-05-28/aya-shouoto-ends-kagetoki-sama-no-kurenai-kokyu-manga-launches-the-demon-prince-of-momochi-house-/.198530</t>
+  </si>
+  <si>
+    <t>The Demon Prince of Momochi House sequel manga launches on July 24</t>
+  </si>
+  <si>
+    <t>The Eminence in Shadow 2nd Season's 2nd Video Reveals More Cast, October 12 Debut, 12-Episode Length</t>
+  </si>
+  <si>
+    <t>https://www.animenewsnetwork.com/news/2023-05-28/the-eminence-in-shadow-2nd-season-2nd-video-reveals-more-cast-october-debut-12-episode-length/.198547</t>
+  </si>
+  <si>
+    <t>Tsuyoshi Koyama, Shizuka Itou, Tomokazu Sugita, Ai Kakuma join cast</t>
+  </si>
+  <si>
+    <t>Knight of the Ice's Yayoi Ogawa Launches New Manga</t>
+  </si>
+  <si>
+    <t>https://www.animenewsnetwork.com/news/2023-05-28/knight-of-the-ice-yayoi-ogawa-launches-new-manga/.198533</t>
+  </si>
+  <si>
+    <t>Eme to Hime launches on June 23</t>
+  </si>
+  <si>
+    <t>K MANGA's Launch Lineup Includes 30+ Manga With English Debuts in U.S.</t>
+  </si>
+  <si>
+    <t>https://www.animenewsnetwork.com/news/2023-05-27/k-manga-launch-lineup-includes-30-manga-with-english-debuts-in-u.s/.198036</t>
+  </si>
+  <si>
+    <t>capeta, Baby Steps, Tomodachi Game, Ace of the Diamond Act II, more debut in English on new service</t>
+  </si>
+  <si>
+    <t>Marvelous Unveils Project Magia Game With Designs by Fairy Tail's Hiro Mashima</t>
+  </si>
+  <si>
+    <t>https://www.animenewsnetwork.com/news/2023-05-26/marvelous-unveils-project-magia-game-with-designs-by-fairy-tail-hiro-mashima/.198463</t>
+  </si>
+  <si>
+    <t>Game's theme is "A New Frontier"</t>
+  </si>
+  <si>
+    <t>Crunchyroll Adds Tenchi Muyo! GXP Paradise Starting Anime</t>
+  </si>
+  <si>
+    <t>https://www.animenewsnetwork.com/news/2023-05-26/crunchyroll-adds-tenchi-muyo-gxp-paradise-starting-anime/.198490</t>
+  </si>
+  <si>
+    <t>3-episode OVA ships as BD in Japan on May 26, June 30, July 28</t>
+  </si>
+  <si>
+    <t>Deathbound Duke's Daughter's Manga Adaptation Ends</t>
+  </si>
+  <si>
+    <t>https://www.animenewsnetwork.com/news/2023-05-28/deathbound-duke-daughter-manga-adaptation-ends/.198531</t>
+  </si>
+  <si>
+    <t>Adaptation of isekai fantasy novel series launched in June 2020</t>
   </si>
   <si>
     <t>Forever Entertainment Delays Launch of Front Mission 2: Remake Game</t>
@@ -213,13 +493,22 @@
     <t>Game was previously slated for release for Switch in June</t>
   </si>
   <si>
-    <t>Yen Press Reveals New Licenses Including Kana Akatsuki's Award-Winning Agent of the Four Seasons Novel</t>
-  </si>
-  <si>
-    <t>https://www.animenewsnetwork.com/news/2023-05-27/yen-press-reveals-new-licenses-including-kana-akatsuki-award-winning-agent-of-the-four-seasons-novel/.198529</t>
-  </si>
-  <si>
-    <t>Fruits Basket artbook, Higurashi When They Cry: GOU anthology, more licensed</t>
+    <t>The Eminence in Shadow: Master of Garden Game Launches for PC with Cross-Platform Play</t>
+  </si>
+  <si>
+    <t>https://www.animenewsnetwork.com/news/2023-05-25/the-eminence-in-shadow-master-of-garden-game-launches-for-pc-with-cross-platform-play/.198443</t>
+  </si>
+  <si>
+    <t>PC game joins iOS/Android versions on Thursday</t>
+  </si>
+  <si>
+    <t>Square Enix Reveals New Dragon Quest Monsters Game for Series' 25th Anniversary</t>
+  </si>
+  <si>
+    <t>https://www.animenewsnetwork.com/news/2023-05-26/square-enix-reveals-new-dragon-quest-monsters-game-for-series-25th-anniversary/.198505</t>
+  </si>
+  <si>
+    <t>New game in development for Switch</t>
   </si>
   <si>
     <t>Mita Ori Launches Our Dining Table Sequel Manga</t>
@@ -231,15 +520,6 @@
     <t>Bokura no Shokutaku: Okawari launched on March 22</t>
   </si>
   <si>
-    <t>K MANGA's Launch Lineup Includes 30+ Manga With English Debuts in U.S.</t>
-  </si>
-  <si>
-    <t>https://www.animenewsnetwork.com/news/2023-05-27/k-manga-launch-lineup-includes-30-manga-with-english-debuts-in-u.s/.198036</t>
-  </si>
-  <si>
-    <t>capeta, Baby Steps, Tomodachi Game, Ace of the Diamond Act II, more debut in English on new service</t>
-  </si>
-  <si>
     <t>Japanese Animation TV Ranking, May 15-21</t>
   </si>
   <si>
@@ -627,345 +907,23 @@
     <t>Story featured in trailer</t>
   </si>
   <si>
-    <t>Dragon's Dogma 2 Game's Trailer Reveals PS5, Xbox Series X|S, Steam Release</t>
-  </si>
-  <si>
-    <t>https://www.animenewsnetwork.com/news/2023-05-24/dragon-dogma-2-game-trailer-reveals-ps5-xbox-series-x-s-steam-release/.198409</t>
-  </si>
-  <si>
-    <t>Gameplay footage shown in trailer</t>
-  </si>
-  <si>
-    <t>Resident Evil 4 Remake VR Mode Trailer Posted</t>
-  </si>
-  <si>
-    <t>https://www.animenewsnetwork.com/news/2023-05-24/resident-evil-4-remake-vr-mode-trailer-posted/.198408</t>
-  </si>
-  <si>
-    <t>Free VR mode update will be available for PS VR2 device on PS5</t>
-  </si>
-  <si>
-    <t>Square Enix Unveils FOAMSTARS 4v4 Multiplayer Shooter</t>
-  </si>
-  <si>
-    <t>https://www.animenewsnetwork.com/news/2023-05-24/square-enix-unveils-foamstars-4v4-multiplayer-shooter/.198407</t>
-  </si>
-  <si>
-    <t>Game slated for PS5/PS4</t>
-  </si>
-  <si>
-    <t>Penguin Box's Odekake Kozame Manga About Young Shark Gets Anime</t>
-  </si>
-  <si>
-    <t>https://www.animenewsnetwork.com/news/2023-05-24/penguin-box-odekake-kozame-manga-about-young-shark-gets-anime/.198394</t>
-  </si>
-  <si>
-    <t>Promo video, visual unveiled</t>
-  </si>
-  <si>
-    <t>Shakugan no Shana Light Novels Get 1st New Volume in 11 Years</t>
-  </si>
-  <si>
-    <t>https://www.animenewsnetwork.com/news/2023-05-23/shakugan-no-shana-light-novels-get-1st-new-volume-in-11-years/.198348</t>
-  </si>
-  <si>
-    <t>New volume is 4th Shakugan no Shana S short story collection</t>
-  </si>
-  <si>
-    <t>Attack on Titan The Final Season Part 3 Anime's 2nd Half Reveals New Visual</t>
-  </si>
-  <si>
-    <t>https://www.animenewsnetwork.com/daily-briefs/2023-05-21/attack-on-titan-the-final-season-part-3-anime-2nd-half-reveals-new-visual/.198260</t>
-  </si>
-  <si>
-    <t>The MAPPA Stage 2023 event on Sunday revealed a new visual for the second half of the Attack on Titan The Final Season Part 3 (Shingeki no Kyojin The Final Season Kanketsu-hen) anime. The second half will premiere this fall. The first half aired as a one-hour special on March 3 (effectively, March 4 in Japan). Crunchyroll streamed the first half under the title Attack on Titan Final Season The Fin...</t>
-  </si>
-  <si>
-    <t>'Reborn as a Vending Machine, I Now Wander the Dungeon' Anime's Full Promo Video Reveals More Cast &amp; Staff, Opening Song, July 5 Debut</t>
-  </si>
-  <si>
-    <t>https://www.animenewsnetwork.com/news/2023-05-24/reborn-as-a-vending-machine-i-now-wander-the-dungeon-anime-full-promo-video-reveals-more-cast-and-/.198391</t>
-  </si>
-  <si>
-    <t>Shiki Aoki, Miyu Tomita, Kazuya Nakai, Ai Kayano, more join isekai fantasy</t>
-  </si>
-  <si>
-    <t>Quintessential Quintuplets' Negi Haruba Designs Original Anime Pon no Michi</t>
-  </si>
-  <si>
-    <t>https://www.animenewsnetwork.com/news/2023-05-23/quintessential-quintuplets-negi-haruba-designs-original-anime-pon-no-michi/.198352</t>
-  </si>
-  <si>
-    <t>OLM's January anime about girls turning mahjong parlor into their hangout</t>
-  </si>
-  <si>
-    <t>Saint Seiya Manga's Live-Action Knights of the Zodiac Film Crosses US$920,000 in U.S. Box Office</t>
-  </si>
-  <si>
-    <t>https://www.animenewsnetwork.com/news/2023-05-22/saint-seiya-manga-live-action-knights-of-the-zodiac-film-crosses-usd920000-in-u.s-box-office/.198312</t>
-  </si>
-  <si>
-    <t>Film debuted in U.S. on May 12</t>
-  </si>
-  <si>
-    <t>Metal Gear Solid 3: Snake Eater Game Gets Remake for PS5</t>
-  </si>
-  <si>
-    <t>https://www.animenewsnetwork.com/news/2023-05-24/metal-gear-solid-3-snake-eater-game-gets-remake-for-ps5/.198405</t>
-  </si>
-  <si>
-    <t>Metal Gear Solid △: Snake Eater, Metal Gear Solid: Master Collection Volume 1 announced</t>
-  </si>
-  <si>
-    <t>Sagu Aoyama, Kintsuba's Spicy Days! Manga Ends With Next Chapter</t>
-  </si>
-  <si>
-    <t>https://www.animenewsnetwork.com/news/2023-05-24/sagu-aoyama-kintsuba-spicy-days-manga-ends-with-next-chapter/.198389</t>
-  </si>
-  <si>
-    <t>Manga about island girls, curry launched in 2021</t>
-  </si>
-  <si>
-    <t>Yoshitaka Ushiki's Oikaze no Jin Manga Ends With Next Chapter</t>
-  </si>
-  <si>
-    <t>https://www.animenewsnetwork.com/news/2023-05-24/yoshitaka-ushiki-oikaze-no-jin-manga-ends-with-next-chapter/.198392</t>
-  </si>
-  <si>
-    <t>Manga about young delivery man launched in July 2021</t>
-  </si>
-  <si>
-    <t>Saru Hashino Launches Toku Touken Ranbu: Hanamaru ~Setsugetsuka~ Anime Film's Manga Adaptation</t>
-  </si>
-  <si>
-    <t>https://www.animenewsnetwork.com/news/2023-05-24/saru-hashino-launches-toku-touken-ranbu-hanamaru-~setsugetsuka~-anime-film-manga-adaptation/.198393</t>
-  </si>
-  <si>
-    <t>First chapter published on Wednesday</t>
-  </si>
-  <si>
-    <t>Demon Slayer: Swordsmith Village Arc Anime's English Dub Debuts on May 28</t>
-  </si>
-  <si>
-    <t>https://www.animenewsnetwork.com/news/2023-05-24/demon-slayer-swordsmith-village-arc-anime-english-dub-debuts-on-may-28/.198382</t>
-  </si>
-  <si>
-    <t>Crunchyroll posts trailer for dub</t>
-  </si>
-  <si>
-    <t>BanG Dream! It's MyGo!!!!! Anime Premieres With 3 Episodes on June 29</t>
-  </si>
-  <si>
-    <t>https://www.animenewsnetwork.com/news/2023-05-24/bang-dream-its-mygo-anime-premieres-with-3-episodes-on-june-29/.198395</t>
-  </si>
-  <si>
-    <t>Videos, theme songs, visual unveiled</t>
-  </si>
-  <si>
-    <t>Soaring Sky! Pretty Cure Anime Gets Puzzle Game Collection on Switch on August 10</t>
-  </si>
-  <si>
-    <t>https://www.animenewsnetwork.com/news/2023-05-24/soaring-sky-pretty-cure-anime-gets-puzzle-game-collection-on-switch-on-august-10/.198376</t>
-  </si>
-  <si>
-    <t>Hirogaru Sky! Precure Hirogaru! Puzzle Collection contains mini games</t>
-  </si>
-  <si>
-    <t>Harvest Moon: The Winds of Anthos Game Launches on September 26</t>
-  </si>
-  <si>
-    <t>https://www.animenewsnetwork.com/news/2023-05-23/harvest-moon-the-winds-of-anthos-game-launches-on-september-26/.198370</t>
-  </si>
-  <si>
-    <t>Game launches on Switch, PS5, PS4, Xbox Series X|S, Xbox One, PC via Steam</t>
-  </si>
-  <si>
-    <t>Hiroyuki's 'Girlfriend, Girlfriend' Manga Ends on May 24 (Updated)</t>
-  </si>
-  <si>
-    <t>https://www.animenewsnetwork.com/news/2023-04-13/hiroyuki-girlfriend-girlfriend-manga-ends-on-may-24/.197037</t>
-  </si>
-  <si>
-    <t>Manga also takes break in Weekly Shōnen Magazine's next issue</t>
-  </si>
-  <si>
-    <t>Demon Slayer: Swordsmith Village Arc Anime Casts Kōichi Yamadera as Zohakuten</t>
-  </si>
-  <si>
-    <t>https://www.animenewsnetwork.com/news/2023-05-21/demon-slayer-swordsmith-village-arc-anime-casts-koichi-yamadera-as-zohakuten/.198294</t>
-  </si>
-  <si>
-    <t>New visual for anime also unveiled</t>
-  </si>
-  <si>
-    <t>The 6th Loop: I'm Finally Free of Auto Mode in this Otome Game Manga Ends with 6th Volume</t>
-  </si>
-  <si>
-    <t>https://www.animenewsnetwork.com/news/2023-05-23/the-6th-loop-im-finally-free-of-auto-mode-in-this-otome-game-manga-ends-with-6th-volume/.198351</t>
-  </si>
-  <si>
-    <t>Isekai fantasy-otome game manga launched in 2020</t>
-  </si>
-  <si>
-    <t>Kodansha USA Licenses A Kingdom of Quartz Manga</t>
-  </si>
-  <si>
-    <t>https://www.animenewsnetwork.com/news/2023-05-23/kodansha-usa-licenses-a-kingdom-of-quartz-manga/.198360</t>
-  </si>
-  <si>
-    <t>BOMHAT's manga debuts in English in spring 2024</t>
-  </si>
-  <si>
-    <t>Saki, Final Fantasy XIV Collaboration Mahjong Manga Ends with 2nd Volume</t>
-  </si>
-  <si>
-    <t>https://www.animenewsnetwork.com/news/2023-05-23/saki-final-fantasy-xiv-collaboration-mahjong-manga-ends-with-2nd-volume/.198349</t>
-  </si>
-  <si>
-    <t>Manga's final volume ships on July 25</t>
-  </si>
-  <si>
-    <t>Frieren: Beyond Journey's End Series Gets 5 1-Shot Spinoff Manga</t>
-  </si>
-  <si>
-    <t>https://www.animenewsnetwork.com/news/2023-05-23/frieren-beyond-journey-end-series-gets-5-1-shot-spinoff-manga/.198347</t>
-  </si>
-  <si>
-    <t>Sunday Webry website launches 1 spinoff manga daily from Monday to Friday</t>
-  </si>
-  <si>
-    <t>Hideo Kojima – Connecting Worlds Documentary Debuts at Tribeca Film Festival on June 17</t>
-  </si>
-  <si>
-    <t>https://www.animenewsnetwork.com/news/2023-05-23/hideo-kojima-connecting-worlds-documentary-debuts-at-tribeca-film-festival-on-june-17/.198356</t>
-  </si>
-  <si>
-    <t>Metal Gear Solid, Death Stranding director participates in extended Q&amp;A session at screening</t>
-  </si>
-  <si>
-    <t>Caressing My Hibernating Bear Anime Reveals English Dub Cast</t>
-  </si>
-  <si>
-    <t>https://www.animenewsnetwork.com/news/2023-05-23/caressing-my-hibernating-bear-anime-reveals-english-dub-cast/.198353</t>
-  </si>
-  <si>
-    <t>BL anime debuted in July 2022</t>
-  </si>
-  <si>
-    <t>Short Shorts Film Festival &amp; Asia 2023 Event Virtually Screens Animated Shorts Until July 10</t>
-  </si>
-  <si>
-    <t>https://www.animenewsnetwork.com/news/2023-05-23/short-shorts-film-festival-and-asia-2023-event-virtually-screens-animated-shorts-until-july-10/.198336</t>
-  </si>
-  <si>
-    <t>14 animated short films by Japanese creators stream worldwide for free</t>
-  </si>
-  <si>
-    <t>Blue Protocol Online Action RPG Launches in Japan on June 14, Delayed in West to 2024 (Updated)</t>
-  </si>
-  <si>
-    <t>https://www.animenewsnetwork.com/daily-briefs/2023-05-23/blue-protocol-online-action-rpg-launches-in-japan-on-june-14-delayed-in-west-to-2024/.198357</t>
-  </si>
-  <si>
-    <t>Bandai Namco announced on Tuesday that Project Sky Blue's multiplayer online action role-playing game Blue Protocol will launch for PC on June 14 in Japan. The service's start time will be revealed at a later date. Pre-registration is now available. Update: Bandai Namco also announced that the game has been delayed in the West to 2024. The game was originally scheduled to launch globally for free ...</t>
-  </si>
-  <si>
-    <t>Undead Girl Murder Farce Anime Casts Reina Kondo</t>
-  </si>
-  <si>
-    <t>https://www.animenewsnetwork.com/news/2023-05-23/undead-girl-murder-farce-anime-casts-reina-kondo/.198355</t>
-  </si>
-  <si>
-    <t>Kondo plays vampire Carmilla in July anime</t>
-  </si>
-  <si>
-    <t>The Super Mario Bros. Movie Becomes #3 Animated Film of All-Time Globally</t>
-  </si>
-  <si>
-    <t>https://www.animenewsnetwork.com/news/2023-05-22/the-super-mario-bros-movie-becomes-no.3-animated-film-of-all-time-globally/.198309</t>
-  </si>
-  <si>
-    <t>Film earns estimated US$16,531,705, stays at #2 in its 7th weekend in the U.S. box office</t>
-  </si>
-  <si>
-    <t>Classroom for Heroes Anime's New Video Reveals More Cast</t>
-  </si>
-  <si>
-    <t>https://www.animenewsnetwork.com/news/2023-05-21/classroom-for-heroes-anime-new-video-reveals-more-cast/.198298</t>
-  </si>
-  <si>
-    <t>Eri Yukimura, Haruka Shiraishi, Sarah Emi Bridcutt, Aya Uchida, 6 more join cast</t>
-  </si>
-  <si>
-    <t>Bocchi the Rock! Anime Gets Compilation Film Next Spring</t>
-  </si>
-  <si>
-    <t>https://www.animenewsnetwork.com/news/2023-05-21/bocchi-the-rock-anime-gets-compilation-film-next-spring/.198288</t>
-  </si>
-  <si>
-    <t>TV anime of Aki Hamaji's 4-panel manga aired last fall</t>
-  </si>
-  <si>
-    <t>Toei, France's La Cachette Collaborate on Le College Noir Animation</t>
-  </si>
-  <si>
-    <t>https://www.animenewsnetwork.com/news/2023-05-23/toei-france-la-cachette-collaborate-on-le-college-noir-animation/.198354</t>
-  </si>
-  <si>
-    <t>Based on Ulysse Malassagne's comic of 5 youths finding missing friend in mountain forests</t>
-  </si>
-  <si>
-    <t>IDOLiSH 7 Franchise's Theatrical Anime Streams Opening Concert Scene</t>
-  </si>
-  <si>
-    <t>https://www.animenewsnetwork.com/news/2023-05-23/idolish-7-franchise-theatrical-anime-streams-opening-concert-scene/.198337</t>
-  </si>
-  <si>
-    <t>Scene features "MONSTER GENERATiON" song</t>
-  </si>
-  <si>
-    <t>Ōoku: The Inner Chambers Anime's English-Subtitled Trailer Reveals June 29 Debut</t>
-  </si>
-  <si>
-    <t>https://www.animenewsnetwork.com/news/2023-05-22/ooku-the-inner-chambers-anime-english-subtitled-trailer-reveals-june-29-debut/.198341</t>
-  </si>
-  <si>
-    <t>Noriyuki Abe directs anime at Studio DEEN</t>
-  </si>
-  <si>
-    <t>Liar Liar Anime Reveals July 8 Premiere Date</t>
-  </si>
-  <si>
-    <t>https://www.animenewsnetwork.com/daily-briefs/2023-05-22/liar-liar-anime-reveals-july-8-premiere-date/.198302</t>
-  </si>
-  <si>
-    <t>The official website for the anime of Haruki Kuō's Liar Liar (not related to Renjuro Kindaichi's Liar x Liar manga) light novel series revealed the anime's July 8 premiere date on Monday. The anime will premiere on Tokyo MX and Sun TV on July 8 at 10:30 p.m. (9:30 a.m. EDT), and on BS Asahi on July 9. The "academy x mind game x romantic comedy" story is set on the "Academy" island where students b...</t>
-  </si>
-  <si>
-    <t>The Fox's Kiss/Black Marriage's Saki Aikawa Launches New Manga</t>
-  </si>
-  <si>
-    <t>https://www.animenewsnetwork.com/news/2023-05-22/the-fox-kiss-black-marriage-saki-aikawa-launches-new-manga/.198287</t>
-  </si>
-  <si>
-    <t>Nidome no Koi wa, Hayami-kun to manga launches on June 5</t>
-  </si>
-  <si>
     <t>Author</t>
   </si>
   <si>
     <t>Comment</t>
   </si>
   <si>
-    <t>Abysswatcherbel</t>
-  </si>
-  <si>
-    <t xml:space="preserve">&amp;gt;This is the place! \(and has been for a year now\)
-Happy birthday thread!
-Also this kills the chance of Secelia dote tomorrow, rip</t>
-  </si>
-  <si>
-    <t>https://www.reddit.com/r/anime/comments/13t3fba/anime_questions_recommendations_and_discussion/jltc39n/</t>
+    <t>AnimeMod</t>
+  </si>
+  <si>
+    <t xml:space="preserve">
+Hello /r/anime, a new daily thread has been posted! Please follow
+[this link](/r/anime/comments/13twlqm/anime_questions_recommendations_and_discussion/) to move on to the new thread
+or [search for the latest thread](/r/anime/search?q=flair%3ADaily&amp;amp;restrict_sr=on&amp;amp;sort=new).
+[](#heartbot "And don't forget to be nice to new users!")</t>
+  </si>
+  <si>
+    <t>https://www.reddit.com/r/anime/comments/13t3fba/anime_questions_recommendations_and_discussion/jlxel6f/</t>
   </si>
   <si>
     <t>alotmorealots</t>
@@ -981,32 +939,6 @@
     <t>https://www.reddit.com/r/anime/comments/13t3fba/anime_questions_recommendations_and_discussion/jlu02b8/</t>
   </si>
   <si>
-    <t>WeeziMonkey</t>
-  </si>
-  <si>
-    <t>Tfw you planned to eat your dinner during the new Jigokuraku episode only to find out it's delayed</t>
-  </si>
-  <si>
-    <t>https://www.reddit.com/r/anime/comments/13t3fba/anime_questions_recommendations_and_discussion/jlu05rv/</t>
-  </si>
-  <si>
-    <t>Watching Danmachi for the first time. Seeing a fantasy RPG world with an adventurer main character not start with reincarnation in the first 5 minutes, my thought was "wait, that's illegal".</t>
-  </si>
-  <si>
-    <t>https://www.reddit.com/r/anime/comments/13t3fba/anime_questions_recommendations_and_discussion/jlu6eln/</t>
-  </si>
-  <si>
-    <t>Krippled_kun</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Holy shit Macross: Do You Remember Love? was spectacular. Fucking blew away all my expectations. Initially thought that Macross: Do You Remember Love? was a summary/compilation of the original Macross series in movie form. But damn that was not the correct assessment. Improved on pretty much every aspect of the original: animation was on steroids, the theme is a fucking banger, the romance felt so much better, and characters  generally felt much more well written. The ending 15 minutes were so \*chefs kiss\*. 
-Was originally gonna skip this movie to move on to the Macross Plus since I've heard great things about Macross Plus' production. Thank god I didn't skip or I would've ended up being a disgrace of a mecha fan. 
-Bravo to Kawamori Shouji and the rest of the staff. So fucking excited now to watch the rest of the franchise.</t>
-  </si>
-  <si>
-    <t>https://www.reddit.com/r/anime/comments/13t3fba/anime_questions_recommendations_and_discussion/jlugqfb/</t>
-  </si>
-  <si>
     <t>KendotsX</t>
   </si>
   <si>
@@ -1018,6 +950,15 @@
     <t>https://www.reddit.com/r/anime/comments/13t3fba/anime_questions_recommendations_and_discussion/jlt2p4q/</t>
   </si>
   <si>
+    <t>WeeziMonkey</t>
+  </si>
+  <si>
+    <t>Watching Danmachi for the first time. Seeing a fantasy RPG world with an adventurer main character not start with reincarnation in the first 5 minutes, my thought was "wait, that's illegal".</t>
+  </si>
+  <si>
+    <t>https://www.reddit.com/r/anime/comments/13t3fba/anime_questions_recommendations_and_discussion/jlu6eln/</t>
+  </si>
+  <si>
     <t>MyrnaMountWeazel</t>
   </si>
   <si>
@@ -1027,6 +968,16 @@
   </si>
   <si>
     <t>https://www.reddit.com/r/anime/comments/13t3fba/anime_questions_recommendations_and_discussion/jltwfn6/</t>
+  </si>
+  <si>
+    <t>SMSmith230</t>
+  </si>
+  <si>
+    <t xml:space="preserve">&amp;gt;[This is the place! (and has been for a year now)](https://preview.redd.it/pdy3s9tkm72b1.png?width=1920&amp;amp;format=png&amp;amp;auto=webp&amp;amp;v=enabled&amp;amp;s=2816a6749e809f9dd216b0e159d7e4061db328ef)
+Death Flag activated!</t>
+  </si>
+  <si>
+    <t>https://www.reddit.com/r/anime/comments/13t3fba/anime_questions_recommendations_and_discussion/jlt3ydj/</t>
   </si>
   <si>
     <t>Massaman95</t>
@@ -1056,16 +1007,6 @@
     <t>https://www.reddit.com/r/anime/comments/13t3fba/anime_questions_recommendations_and_discussion/jlt367k/</t>
   </si>
   <si>
-    <t>SMSmith230</t>
-  </si>
-  <si>
-    <t xml:space="preserve">&amp;gt;[This is the place! (and has been for a year now)](https://preview.redd.it/pdy3s9tkm72b1.png?width=1920&amp;amp;format=png&amp;amp;auto=webp&amp;amp;v=enabled&amp;amp;s=2816a6749e809f9dd216b0e159d7e4061db328ef)
-Death Flag activated!</t>
-  </si>
-  <si>
-    <t>https://www.reddit.com/r/anime/comments/13t3fba/anime_questions_recommendations_and_discussion/jlt3ydj/</t>
-  </si>
-  <si>
     <t>baboon_bassoon</t>
   </si>
   <si>
@@ -1073,6 +1014,26 @@
   </si>
   <si>
     <t>https://www.reddit.com/r/anime/comments/13t3fba/anime_questions_recommendations_and_discussion/jltejwd/</t>
+  </si>
+  <si>
+    <t>LimeyLassen</t>
+  </si>
+  <si>
+    <t>Any Tearmoon Empire enjoyers? I'm really looking forward to the anime adapation, it looks high quality.</t>
+  </si>
+  <si>
+    <t>https://www.reddit.com/r/anime/comments/13t3fba/anime_questions_recommendations_and_discussion/jlwlm53/</t>
+  </si>
+  <si>
+    <t>Abysswatcherbel</t>
+  </si>
+  <si>
+    <t xml:space="preserve">&amp;gt;This is the place! \(and has been for a year now\)
+Happy birthday thread!
+Also this kills the chance of Secelia dote tomorrow, rip</t>
+  </si>
+  <si>
+    <t>https://www.reddit.com/r/anime/comments/13t3fba/anime_questions_recommendations_and_discussion/jltc39n/</t>
   </si>
   <si>
     <t>yorocky89A</t>
@@ -1107,31 +1068,15 @@
     <t>https://www.reddit.com/r/anime/comments/13t3fba/anime_questions_recommendations_and_discussion/jltoo8r/</t>
   </si>
   <si>
-    <t>ThisShitisDope</t>
-  </si>
-  <si>
-    <t>Bocchi the Rock's new song [Into the Light with translation](https://www.youtube.com/watch?v=pCe6Bq739qQ) has got me ecstatic in my 12 am reverie. I can't count how many BtR has made me cry already.</t>
-  </si>
-  <si>
-    <t>https://www.reddit.com/r/anime/comments/13t3fba/anime_questions_recommendations_and_discussion/jlvpdpp/</t>
-  </si>
-  <si>
-    <t>LimeyLassen</t>
-  </si>
-  <si>
-    <t>Any Tearmoon Empire enjoyers? I'm really looking forward to the anime adapation, it looks high quality.</t>
-  </si>
-  <si>
-    <t>https://www.reddit.com/r/anime/comments/13t3fba/anime_questions_recommendations_and_discussion/jlwlm53/</t>
-  </si>
-  <si>
-    <t>QuanxiEnjoyer247</t>
-  </si>
-  <si>
-    <t>Hello my fellow Anime Enjoyers. If there are any Germans among you id like to ask where you buy your merch? Id love to start getting into it a bit so anything from shirts, stickers, figures and so on or actual Manga and Blue-Rays as well : ) I struggle to find good online Stories so id appreciate any help I can get. Enjoy your Weekend</t>
-  </si>
-  <si>
-    <t>https://www.reddit.com/r/anime/comments/13t3fba/anime_questions_recommendations_and_discussion/jlt57dx/</t>
+    <t>Krippled_kun</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Holy shit Macross: Do You Remember Love? was spectacular. Fucking blew away all my expectations. Initially thought that Macross: Do You Remember Love? was a summary/compilation of the original Macross series in movie form. But damn that was not the correct assessment. Improved on pretty much every aspect of the original: animation was on steroids, the theme is a fucking banger, the romance felt so much better, and characters  generally felt much more well written. The ending 15 minutes were so \*chefs kiss\*. 
+Was originally gonna skip this movie to move on to the Macross Plus since I've heard great things about Macross Plus' production. Thank god I didn't skip or I would've ended up being a disgrace of a mecha fan. 
+Bravo to Kawamori Shouji and the rest of the staff. So fucking excited now to watch the rest of the franchise.</t>
+  </si>
+  <si>
+    <t>https://www.reddit.com/r/anime/comments/13t3fba/anime_questions_recommendations_and_discussion/jlugqfb/</t>
   </si>
   <si>
     <t>LoanGrahamXCarkeys</t>
@@ -1144,6 +1089,40 @@
     <t>https://www.reddit.com/r/anime/comments/13t3fba/anime_questions_recommendations_and_discussion/jltabg0/</t>
   </si>
   <si>
+    <t>TheRedForever</t>
+  </si>
+  <si>
+    <t xml:space="preserve">For you Macross fans in the U.S., the theater list for the June 4th Walkure final concert has been posted on the Live Viewing Japan website.  
+https://liveviewing.jp/overseas/walkure-lastmission-eng/</t>
+  </si>
+  <si>
+    <t>https://www.reddit.com/r/anime/comments/13t3fba/anime_questions_recommendations_and_discussion/jlw0ix2/</t>
+  </si>
+  <si>
+    <t>Tfw you planned to eat your dinner during the new Jigokuraku episode only to find out it's delayed</t>
+  </si>
+  <si>
+    <t>https://www.reddit.com/r/anime/comments/13t3fba/anime_questions_recommendations_and_discussion/jlu05rv/</t>
+  </si>
+  <si>
+    <t>Larielia</t>
+  </si>
+  <si>
+    <t>What shows are similar to the Atelier games?</t>
+  </si>
+  <si>
+    <t>https://www.reddit.com/r/anime/comments/13t3fba/anime_questions_recommendations_and_discussion/jltzbxq/</t>
+  </si>
+  <si>
+    <t>QuanxiEnjoyer247</t>
+  </si>
+  <si>
+    <t>Hello my fellow Anime Enjoyers. If there are any Germans among you id like to ask where you buy your merch? Id love to start getting into it a bit so anything from shirts, stickers, figures and so on or actual Manga and Blue-Rays as well : ) I struggle to find good online Stories so id appreciate any help I can get. Enjoy your Weekend</t>
+  </si>
+  <si>
+    <t>https://www.reddit.com/r/anime/comments/13t3fba/anime_questions_recommendations_and_discussion/jlt57dx/</t>
+  </si>
+  <si>
     <t>KaleidoArachnid</t>
   </si>
   <si>
@@ -1154,6 +1133,33 @@
     <t>https://www.reddit.com/r/anime/comments/13t3fba/anime_questions_recommendations_and_discussion/jltet6r/</t>
   </si>
   <si>
+    <t>jojoismyreligion</t>
+  </si>
+  <si>
+    <t>I'm 30 episodes into Gintama. It's been episodic so far. When does longer arcs come around ?</t>
+  </si>
+  <si>
+    <t>https://www.reddit.com/r/anime/comments/13t3fba/anime_questions_recommendations_and_discussion/jltormf/</t>
+  </si>
+  <si>
+    <t>Emergency-Pineapples</t>
+  </si>
+  <si>
+    <t>Does Gintama have any character development at any point?</t>
+  </si>
+  <si>
+    <t>https://www.reddit.com/r/anime/comments/13t3fba/anime_questions_recommendations_and_discussion/jlu0hyn/</t>
+  </si>
+  <si>
+    <t>ThisShitisDope</t>
+  </si>
+  <si>
+    <t>Bocchi the Rock's new song [Into the Light with translation](https://www.youtube.com/watch?v=pCe6Bq739qQ) has got me ecstatic in my 12 am reverie. I can't count how many BtR has made me cry already.</t>
+  </si>
+  <si>
+    <t>https://www.reddit.com/r/anime/comments/13t3fba/anime_questions_recommendations_and_discussion/jlvpdpp/</t>
+  </si>
+  <si>
     <t>soberdruguser</t>
   </si>
   <si>
@@ -1163,50 +1169,13 @@
     <t>https://www.reddit.com/r/anime/comments/13t3fba/anime_questions_recommendations_and_discussion/jlv6wki/</t>
   </si>
   <si>
-    <t>TheRedForever</t>
-  </si>
-  <si>
-    <t xml:space="preserve">For you Macross fans in the U.S., the theater list for the June 4th Walkure final concert has been posted on the Live Viewing Japan website.  
-https://liveviewing.jp/overseas/walkure-lastmission-eng/</t>
-  </si>
-  <si>
-    <t>https://www.reddit.com/r/anime/comments/13t3fba/anime_questions_recommendations_and_discussion/jlw0ix2/</t>
-  </si>
-  <si>
-    <t>jojoismyreligion</t>
-  </si>
-  <si>
-    <t>I'm 30 episodes into Gintama. It's been episodic so far. When does longer arcs come around ?</t>
-  </si>
-  <si>
-    <t>https://www.reddit.com/r/anime/comments/13t3fba/anime_questions_recommendations_and_discussion/jltormf/</t>
-  </si>
-  <si>
-    <t>Larielia</t>
-  </si>
-  <si>
-    <t>What shows are similar to the Atelier games?</t>
-  </si>
-  <si>
-    <t>https://www.reddit.com/r/anime/comments/13t3fba/anime_questions_recommendations_and_discussion/jltzbxq/</t>
-  </si>
-  <si>
-    <t>Emergency-Pineapples</t>
-  </si>
-  <si>
-    <t>Does Gintama have any character development at any point?</t>
-  </si>
-  <si>
-    <t>https://www.reddit.com/r/anime/comments/13t3fba/anime_questions_recommendations_and_discussion/jlu0hyn/</t>
-  </si>
-  <si>
-    <t>ikarus_77</t>
-  </si>
-  <si>
-    <t>I usually get the animes i watch from shorts on YouTube and amv's i recently saw an amv with Hellsing ultimate so I want to ask if it isn't too dark and how many versions/seasons there are bc i have to plan things i watch or else my sleep schedule is f*ed</t>
-  </si>
-  <si>
-    <t>https://www.reddit.com/r/anime/comments/13t3fba/anime_questions_recommendations_and_discussion/jlt4fzq/</t>
+    <t>Cr4zko</t>
+  </si>
+  <si>
+    <t>Is it just me or anime was better in the 2000s? Gah, just can't find anything that's my groove lately.</t>
+  </si>
+  <si>
+    <t>https://www.reddit.com/r/anime/comments/13t3fba/anime_questions_recommendations_and_discussion/jlvyby4/</t>
   </si>
   <si>
     <t>LoPanDidNothingWrong</t>
@@ -1219,51 +1188,6 @@
     <t>https://www.reddit.com/r/anime/comments/13t3fba/anime_questions_recommendations_and_discussion/jltq3rm/</t>
   </si>
   <si>
-    <t>badcupcakehoarder</t>
-  </si>
-  <si>
-    <t>What anime can you think of that have a non-romance focus plot but romance is one of the main motivation/catalysts for the main character to start the story?</t>
-  </si>
-  <si>
-    <t>https://www.reddit.com/r/anime/comments/13t3fba/anime_questions_recommendations_and_discussion/jlv35kd/</t>
-  </si>
-  <si>
-    <t>Cr4zko</t>
-  </si>
-  <si>
-    <t>Is it just me or anime was better in the 2000s? Gah, just can't find anything that's my groove lately.</t>
-  </si>
-  <si>
-    <t>https://www.reddit.com/r/anime/comments/13t3fba/anime_questions_recommendations_and_discussion/jlvyby4/</t>
-  </si>
-  <si>
-    <t>geargrinder_11</t>
-  </si>
-  <si>
-    <t>Hi! I’m looking for a more chill anime, more slice of life style. More just chilling out anime, like laid back camp, or something similar. Preferably in a modern setting, or flying witch which is a more misadventures of a character(s)</t>
-  </si>
-  <si>
-    <t>https://www.reddit.com/r/anime/comments/13t3fba/anime_questions_recommendations_and_discussion/jlvz5ie/</t>
-  </si>
-  <si>
-    <t>[deleted]</t>
-  </si>
-  <si>
-    <t>[removed]</t>
-  </si>
-  <si>
-    <t>https://www.reddit.com/r/anime/comments/13t3fba/anime_questions_recommendations_and_discussion/jlw8no3/</t>
-  </si>
-  <si>
-    <t>jen___22</t>
-  </si>
-  <si>
-    <t>Can you recommend new anime?</t>
-  </si>
-  <si>
-    <t>https://www.reddit.com/r/anime/comments/13t3fba/anime_questions_recommendations_and_discussion/jlwj657/</t>
-  </si>
-  <si>
     <t>rabnabombshell</t>
   </si>
   <si>
@@ -1271,6 +1195,15 @@
   </si>
   <si>
     <t>https://www.reddit.com/r/anime/comments/13t3fba/anime_questions_recommendations_and_discussion/jlufjq4/</t>
+  </si>
+  <si>
+    <t>RichPen7644</t>
+  </si>
+  <si>
+    <t>Anyone have any good anime recommendations for this season?, I feel like it is getting harder and harder to find a good anime to start</t>
+  </si>
+  <si>
+    <t>https://www.reddit.com/r/anime/comments/13t3fba/anime_questions_recommendations_and_discussion/jlwztq6/</t>
   </si>
   <si>
     <t>NordF150</t>
@@ -1283,6 +1216,382 @@
   </si>
   <si>
     <t>https://www.reddit.com/r/anime/comments/13t3fba/anime_questions_recommendations_and_discussion/jluqou9/</t>
+  </si>
+  <si>
+    <t>ikarus_77</t>
+  </si>
+  <si>
+    <t>I usually get the animes i watch from shorts on YouTube and amv's i recently saw an amv with Hellsing ultimate so I want to ask if it isn't too dark and how many versions/seasons there are bc i have to plan things i watch or else my sleep schedule is f*ed</t>
+  </si>
+  <si>
+    <t>https://www.reddit.com/r/anime/comments/13t3fba/anime_questions_recommendations_and_discussion/jlt4fzq/</t>
+  </si>
+  <si>
+    <t>badcupcakehoarder</t>
+  </si>
+  <si>
+    <t>What anime can you think of that have a non-romance focus plot but romance is one of the main motivation/catalysts for the main character to start the story?</t>
+  </si>
+  <si>
+    <t>https://www.reddit.com/r/anime/comments/13t3fba/anime_questions_recommendations_and_discussion/jlv35kd/</t>
+  </si>
+  <si>
+    <t>geargrinder_11</t>
+  </si>
+  <si>
+    <t>Hi! I’m looking for a more chill anime, more slice of life style. More just chilling out anime, like laid back camp, or something similar. Preferably in a modern setting, or flying witch which is a more misadventures of a character(s)</t>
+  </si>
+  <si>
+    <t>https://www.reddit.com/r/anime/comments/13t3fba/anime_questions_recommendations_and_discussion/jlvz5ie/</t>
+  </si>
+  <si>
+    <t>[deleted]</t>
+  </si>
+  <si>
+    <t>[removed]</t>
+  </si>
+  <si>
+    <t>https://www.reddit.com/r/anime/comments/13t3fba/anime_questions_recommendations_and_discussion/jlw8no3/</t>
+  </si>
+  <si>
+    <t>jen___22</t>
+  </si>
+  <si>
+    <t>Can you recommend new anime?</t>
+  </si>
+  <si>
+    <t>https://www.reddit.com/r/anime/comments/13t3fba/anime_questions_recommendations_and_discussion/jlwj657/</t>
+  </si>
+  <si>
+    <t>FuckinGuiltyGearWeeb</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Anyone have recommendations for romance anime?  
+Off the top my head I've seen, (romance anime)
+Bunny Senpai
+Banished from the heroes party 
+Spice and Wolf 
+Chivalry of a failed knight
+Dropped Vermeil in Gold 
+Kaguya-sama 1st season</t>
+  </si>
+  <si>
+    <t>https://www.reddit.com/r/anime/comments/13t3fba/anime_questions_recommendations_and_discussion/jlwos26/</t>
+  </si>
+  <si>
+    <t>Lychee_fart4236</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Anyone have recommendations for animes with hikikomoris in them? 
+I'm looking for an anime with hikikomoris in them.
+I've watched welcome to the NHK and I love that anime. It's one of my favorites.
+I don't really know if watamote is also considered a hiki, but I watched that one as well and I enjoyed it.</t>
+  </si>
+  <si>
+    <t>https://www.reddit.com/r/anime/comments/13t3fba/anime_questions_recommendations_and_discussion/jlwqygs/</t>
+  </si>
+  <si>
+    <t>Hairy_Departure1</t>
+  </si>
+  <si>
+    <t>Where is [this place](https://i.imgur.com/vMqVldV.jpg) that comes up at the ED in My Love Story with Yamada-kun at Lv999</t>
+  </si>
+  <si>
+    <t>https://www.reddit.com/r/anime/comments/13t3fba/anime_questions_recommendations_and_discussion/jlx12ek/</t>
+  </si>
+  <si>
+    <t>https://www.reddit.comundefined</t>
+  </si>
+  <si>
+    <t>Upvotes</t>
+  </si>
+  <si>
+    <t>Comments</t>
+  </si>
+  <si>
+    <t>Suzume Bags Over 14 Billion Yen; Surpasses Weathering With You</t>
+  </si>
+  <si>
+    <t>suguruscurse</t>
+  </si>
+  <si>
+    <t>https://www.reddit.com/r/animenews/comments/13v7vc4/suzume_bags_over_14_billion_yen_surpasses/</t>
+  </si>
+  <si>
+    <t>Cygames Reveals Bang Brave Bang Bravern Original TV Anime</t>
+  </si>
+  <si>
+    <t>Aggravating-Lead29</t>
+  </si>
+  <si>
+    <t>https://www.reddit.com/r/animenews/comments/13ur4t3/cygames_reveals_bang_brave_bang_bravern_original/</t>
+  </si>
+  <si>
+    <t>https://www.reddit.com/r/animenews/comments/13ur1g3/the_first_slam_dunk_surpasses_weathering_with_you/</t>
+  </si>
+  <si>
+    <t>'Rascal Does Not Dream of a Sister Venturing Out'– Completion Announcement Screening and Release Date Revealed</t>
+  </si>
+  <si>
+    <t>asianlegends</t>
+  </si>
+  <si>
+    <t>https://www.reddit.com/r/animenews/comments/13uonxr/rascal_does_not_dream_of_a_sister_venturing_out/</t>
+  </si>
+  <si>
+    <t>https://www.reddit.com/r/animenews/comments/13uoks5/the_masterful_cat_is_depressed_again_today_anime/</t>
+  </si>
+  <si>
+    <t>The Eminence in Shadow 2nd Season's 2nd Video Reveals More Cast, October Debut, 12-Episode Length</t>
+  </si>
+  <si>
+    <t>https://www.reddit.com/r/animenews/comments/13uf5fo/the_eminence_in_shadow_2nd_seasons_2nd_video/</t>
+  </si>
+  <si>
+    <t>https://www.reddit.com/r/animenews/comments/13uf2si/bleach_thousandyear_blood_war_animes_video/</t>
+  </si>
+  <si>
+    <t>Hajime no Ippo Author Confused by G Gundam Episode 12</t>
+  </si>
+  <si>
+    <t>https://www.reddit.com/r/animenews/comments/13u42ra/hajime_no_ippo_author_confused_by_g_gundam/</t>
+  </si>
+  <si>
+    <t>Megumi Ishitani Rumored To Be Working On Luffy's Gear 5 Episodes</t>
+  </si>
+  <si>
+    <t>https://www.reddit.com/r/animenews/comments/13u26rc/megumi_ishitani_rumored_to_be_working_on_luffys/</t>
+  </si>
+  <si>
+    <t>New Trailer and Key Visual - Bleach Thousand Year Blood War Cour 2 Anime</t>
+  </si>
+  <si>
+    <t>https://www.reddit.com/r/animenews/comments/13tyk0o/new_trailer_and_key_visual_bleach_thousand_year/</t>
+  </si>
+  <si>
+    <t>"Blue Orchestra" Episode 8 Preceding Scene Cut Released</t>
+  </si>
+  <si>
+    <t>https://www.reddit.com/r/animenews/comments/13twgol/blue_orchestra_episode_8_preceding_scene_cut/</t>
+  </si>
+  <si>
+    <t>https://www.reddit.com/r/animenews/comments/13tvn4y/zom_100_bucket_list_of_the_dead_anime_debuts_on/</t>
+  </si>
+  <si>
+    <t>Demon Slayer: Kimetsu no Yaiba Swordsmith Village Arc English Dub Begins May 28</t>
+  </si>
+  <si>
+    <t>realplayer16</t>
+  </si>
+  <si>
+    <t>https://www.reddit.com/r/animenews/comments/13t4uoh/demon_slayer_kimetsu_no_yaiba_swordsmith_village/</t>
+  </si>
+  <si>
+    <t>Michael B Jordan Reveals Why He Declined Offers To Direct Live-Action Adaptations Of Anime</t>
+  </si>
+  <si>
+    <t>Borgasmic_Peeza</t>
+  </si>
+  <si>
+    <t>https://www.reddit.com/r/animenews/comments/13t1ogr/michael_b_jordan_reveals_why_he_declined_offers/</t>
+  </si>
+  <si>
+    <t>Mashle: Magic And Magic Anime Announces Cast For Magia Lupus Organization Members</t>
+  </si>
+  <si>
+    <t>Oatmeel97</t>
+  </si>
+  <si>
+    <t>https://www.reddit.com/r/animenews/comments/13sqbtd/mashle_magic_and_magic_anime_announces_cast_for/</t>
+  </si>
+  <si>
+    <t>Crunchyroll Adds ‘Tenchi Muyo! GXP Paradise’ Anime Streaming</t>
+  </si>
+  <si>
+    <t>https://www.reddit.com/r/animenews/comments/13slv6g/crunchyroll_adds_tenchi_muyo_gxp_paradise_anime/</t>
+  </si>
+  <si>
+    <t>Mushoku Tensei Season 2 Reveals New Trailer, Release Date &amp;amp; Theme Songs</t>
+  </si>
+  <si>
+    <t>https://www.reddit.com/r/animenews/comments/13sc4ju/mushoku_tensei_season_2_reveals_new_trailer/</t>
+  </si>
+  <si>
+    <t>Veteran Mangaka Defends Oshi No Ko Anime Amid Recent Controversy</t>
+  </si>
+  <si>
+    <t>https://www.reddit.com/r/animenews/comments/13sbsez/veteran_mangaka_defends_oshi_no_ko_anime_amid/</t>
+  </si>
+  <si>
+    <t>https://www.reddit.com/r/animenews/comments/13saryp/ai_no_idenshi_scifi_tv_animes_2nd_promo_video/</t>
+  </si>
+  <si>
+    <t>Kyoto Animation To Construct Two Memorials To Honour Arson Attack Victims</t>
+  </si>
+  <si>
+    <t>https://www.reddit.com/r/animenews/comments/13s9apl/kyoto_animation_to_construct_two_memorials_to/</t>
+  </si>
+  <si>
+    <t>https://www.reddit.com/r/animenews/comments/13s9aiw/helck_tv_anime_reveals_promo_video_july_11/</t>
+  </si>
+  <si>
+    <t>https://www.reddit.com/r/animenews/comments/13s9920/ragna_crimson_tv_animes_2nd_promo_video_reveals/</t>
+  </si>
+  <si>
+    <t>https://www.reddit.com/r/animenews/comments/13s4irg/tsuyokute_new_saga_anime_delayed_from_july_2023/</t>
+  </si>
+  <si>
+    <t>https://www.reddit.com/r/animenews/comments/13s3bxl/black_clover_sword_of_the_wizard_king_films/</t>
+  </si>
+  <si>
+    <t>https://www.reddit.com/r/animenews/comments/13s2ezm/kenta_ishizakas_travel_manga_thats_journey_gets/</t>
+  </si>
+  <si>
+    <t>https://www.reddit.com/r/animenews/comments/13rwzl8/delicious_in_dungeon_animes_teaser_trailer/</t>
+  </si>
+  <si>
+    <t>YOASOBI Releases Oshi No Ko Opening “Idol” In English Dub</t>
+  </si>
+  <si>
+    <t>https://www.reddit.com/r/animenews/comments/13rluw5/yoasobi_releases_oshi_no_ko_opening_idol_in/</t>
+  </si>
+  <si>
+    <t>One Piece Live-Action Poster Leaked, Fans Split On Design Changes</t>
+  </si>
+  <si>
+    <t>https://www.reddit.com/r/animenews/comments/13rjp3u/one_piece_liveaction_poster_leaked_fans_split_on/</t>
+  </si>
+  <si>
+    <t>https://www.reddit.com/r/animenews/comments/13rcmda/sugar_apple_fairy_tale_anime_reveals_key_visual/</t>
+  </si>
+  <si>
+    <t>Diego Maradona Declares One Piece The Greatest Anime As His Facebook Account Gets Hacked</t>
+  </si>
+  <si>
+    <t>https://www.reddit.com/r/animenews/comments/13rc1oh/diego_maradona_declares_one_piece_the_greatest/</t>
+  </si>
+  <si>
+    <t>Penguin Box's Odekake Kozame Manga About Young Shark Gets Anime</t>
+  </si>
+  <si>
+    <t>https://www.reddit.com/r/animenews/comments/13r697k/penguin_boxs_odekake_kozame_manga_about_young/</t>
+  </si>
+  <si>
+    <t>Oshi No Ko Episode 6 Gets Criticized For Replicating Deceased Hana Kimura's Cyberbullying Tragedy</t>
+  </si>
+  <si>
+    <t>https://www.reddit.com/r/animenews/comments/13qtp9q/oshi_no_ko_episode_6_gets_criticized_for/</t>
+  </si>
+  <si>
+    <t>Record Of Ragnarok Season 2 Part 2 Release Date, Additional Cast &amp;amp; New Visual Revealed - Anime Explained</t>
+  </si>
+  <si>
+    <t>weebreviews</t>
+  </si>
+  <si>
+    <t>https://www.reddit.com/r/animenews/comments/13qsl2n/record_of_ragnarok_season_2_part_2_release_date/</t>
+  </si>
+  <si>
+    <t>Oshi No Ko Episode 8 Delayed; Recap Episode Will Air On May 31</t>
+  </si>
+  <si>
+    <t>https://www.reddit.com/r/animenews/comments/13qq0hb/oshi_no_ko_episode_8_delayed_recap_episode_will/</t>
+  </si>
+  <si>
+    <t>The First Slam Dunk Anime Movie To Premiere At Anime Expo North America</t>
+  </si>
+  <si>
+    <t>https://www.reddit.com/r/animenews/comments/13ql93y/the_first_slam_dunk_anime_movie_to_premiere_at/</t>
+  </si>
+  <si>
+    <t>'Reborn as a Vending Machine, I Now Wander the Dungeon' Anime's Full Promo Video Reveals More Cast &amp;amp; Staff, Opening Song, July 5 Debut</t>
+  </si>
+  <si>
+    <t>https://www.reddit.com/r/animenews/comments/13qi6ue/reborn_as_a_vending_machine_i_now_wander_the/</t>
+  </si>
+  <si>
+    <t>Quintessential Quintuplets' Negi Haruba Designs Original Anime Pon no Michi</t>
+  </si>
+  <si>
+    <t>https://www.reddit.com/r/animenews/comments/13pngwi/quintessential_quintuplets_negi_haruba_designs/</t>
+  </si>
+  <si>
+    <t>Steins;Gate Live-Action Adaptation Was Scrapped Over Rintarou Okabe's Casting</t>
+  </si>
+  <si>
+    <t>https://www.reddit.com/r/animenews/comments/13pn0fx/steinsgate_liveaction_adaptation_was_scrapped/</t>
+  </si>
+  <si>
+    <t>KamiKatsu: Working For God In A Godless World Episode 8 Release Date Gets Delayed</t>
+  </si>
+  <si>
+    <t>https://www.reddit.com/r/animenews/comments/13pias6/kamikatsu_working_for_god_in_a_godless_world/</t>
+  </si>
+  <si>
+    <t>Ōoku: The Inner Chambers Anime's English-Subtitled Trailer Reveals June 29 Debut</t>
+  </si>
+  <si>
+    <t>https://www.reddit.com/r/animenews/comments/13pcpt2/ōoku_the_inner_chambers_animes_englishsubtitled/</t>
+  </si>
+  <si>
+    <t>Oshi No Ko Anime Accused Of Profiting From Hana Kimura’s Suicide Story</t>
+  </si>
+  <si>
+    <t>https://www.reddit.com/r/animenews/comments/13p3e1p/oshi_no_ko_anime_accused_of_profiting_from_hana/</t>
+  </si>
+  <si>
+    <t>2nd Mr. Osomatsu 6th Anniversary Anime Film Reveals Ending Song Artists</t>
+  </si>
+  <si>
+    <t>https://www.reddit.com/r/animenews/comments/13ooysr/2nd_mr_osomatsu_6th_anniversary_anime_film/</t>
+  </si>
+  <si>
+    <t>Michael B. Jordan Visits Naruto Anime's Production Studio</t>
+  </si>
+  <si>
+    <t>https://www.reddit.com/r/animenews/comments/13oo31p/michael_b_jordan_visits_naruto_animes_production/</t>
+  </si>
+  <si>
+    <t>Final Ultraman CG Anime Season's Special Trailer Highlights Final Ultraman Form</t>
+  </si>
+  <si>
+    <t>https://www.reddit.com/r/animenews/comments/13ohze4/final_ultraman_cg_anime_seasons_special_trailer/</t>
+  </si>
+  <si>
+    <t>Liar Liar Anime Reveals July 8 Premiere Date</t>
+  </si>
+  <si>
+    <t>https://www.reddit.com/r/animenews/comments/13ohv7h/liar_liar_anime_reveals_july_8_premiere_date/</t>
+  </si>
+  <si>
+    <t>Paradox Live The Animation's Teaser Previews 1st Anime Footage</t>
+  </si>
+  <si>
+    <t>https://www.reddit.com/r/animenews/comments/13oadid/paradox_live_the_animations_teaser_previews_1st/</t>
+  </si>
+  <si>
+    <t>Mari Okada, MAPPA's Alice to Therese no Maboroshi Kōjō Anime Film Reveals Cast, Story, Teaser, September 15 Debut</t>
+  </si>
+  <si>
+    <t>https://www.reddit.com/r/animenews/comments/13ntn9q/mari_okada_mappas_alice_to_therese_no_maboroshi/</t>
+  </si>
+  <si>
+    <t>Sunao Katabuchi's New Film Reveals Title, Video, Teaser Visual</t>
+  </si>
+  <si>
+    <t>https://www.reddit.com/r/animenews/comments/13ntmzq/sunao_katabuchis_new_film_reveals_title_video/</t>
+  </si>
+  <si>
+    <t>Banana Fish Director Hiroko Utsumi, MAPPA Unveil Bucchigiri?! TV Anime for January</t>
+  </si>
+  <si>
+    <t>https://www.reddit.com/r/animenews/comments/13ntly6/banana_fish_director_hiroko_utsumi_mappa_unveil/</t>
+  </si>
+  <si>
+    <t>NEW JJK SEASON 2 TRAILER!!!</t>
+  </si>
+  <si>
+    <t>https://www.reddit.com/r/animenews/comments/13nqklx/new_jjk_season_2_trailer/</t>
   </si>
 </sst>
 </file>
@@ -1907,7 +2216,7 @@
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:C84"/>
+  <dimension ref="A1:C79"/>
   <sheetFormatPr defaultRowHeight="15" outlineLevelRow="0" outlineLevelCol="0" x14ac:dyDescent="55"/>
   <cols>
     <col min="1" max="1" width="30" customWidth="1"/>
@@ -2784,61 +3093,6 @@
         <v>296</v>
       </c>
     </row>
-    <row r="80" ht="50" customHeight="1" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A80" t="s">
-        <v>297</v>
-      </c>
-      <c r="B80" t="s">
-        <v>298</v>
-      </c>
-      <c r="C80" t="s">
-        <v>299</v>
-      </c>
-    </row>
-    <row r="81" ht="50" customHeight="1" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A81" t="s">
-        <v>300</v>
-      </c>
-      <c r="B81" t="s">
-        <v>301</v>
-      </c>
-      <c r="C81" t="s">
-        <v>302</v>
-      </c>
-    </row>
-    <row r="82" ht="50" customHeight="1" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A82" t="s">
-        <v>303</v>
-      </c>
-      <c r="B82" t="s">
-        <v>304</v>
-      </c>
-      <c r="C82" t="s">
-        <v>305</v>
-      </c>
-    </row>
-    <row r="83" ht="50" customHeight="1" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A83" t="s">
-        <v>306</v>
-      </c>
-      <c r="B83" t="s">
-        <v>307</v>
-      </c>
-      <c r="C83" t="s">
-        <v>308</v>
-      </c>
-    </row>
-    <row r="84" ht="50" customHeight="1" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A84" t="s">
-        <v>309</v>
-      </c>
-      <c r="B84" t="s">
-        <v>310</v>
-      </c>
-      <c r="C84" t="s">
-        <v>311</v>
-      </c>
-    </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup orientation="portrait" horizontalDpi="4294967295" verticalDpi="4294967295" scale="100" fitToWidth="1" fitToHeight="1"/>
@@ -2847,7 +3101,7 @@
 
 <file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:C34"/>
+  <dimension ref="A1:C40"/>
   <sheetFormatPr defaultRowHeight="15" outlineLevelRow="0" outlineLevelCol="0" x14ac:dyDescent="55"/>
   <cols>
     <col min="1" max="1" width="30" customWidth="1"/>
@@ -2857,10 +3111,10 @@
   <sheetData>
     <row r="1" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A1" t="s">
-        <v>312</v>
+        <v>297</v>
       </c>
       <c r="B1" t="s">
-        <v>313</v>
+        <v>298</v>
       </c>
       <c r="C1" t="s">
         <v>1</v>
@@ -2868,365 +3122,1309 @@
     </row>
     <row r="2" ht="200" customHeight="1" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A2" t="s">
-        <v>314</v>
+        <v>299</v>
       </c>
       <c r="B2" t="s">
-        <v>315</v>
+        <v>300</v>
       </c>
       <c r="C2" t="s">
-        <v>316</v>
+        <v>301</v>
       </c>
     </row>
     <row r="3" ht="200" customHeight="1" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A3" t="s">
-        <v>317</v>
+        <v>302</v>
       </c>
       <c r="B3" t="s">
-        <v>318</v>
+        <v>303</v>
       </c>
       <c r="C3" t="s">
-        <v>319</v>
+        <v>304</v>
       </c>
     </row>
     <row r="4" ht="200" customHeight="1" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A4" t="s">
-        <v>320</v>
+        <v>305</v>
       </c>
       <c r="B4" t="s">
-        <v>321</v>
+        <v>306</v>
       </c>
       <c r="C4" t="s">
-        <v>322</v>
+        <v>307</v>
       </c>
     </row>
     <row r="5" ht="200" customHeight="1" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A5" t="s">
-        <v>320</v>
+        <v>308</v>
       </c>
       <c r="B5" t="s">
-        <v>323</v>
+        <v>309</v>
       </c>
       <c r="C5" t="s">
-        <v>324</v>
+        <v>310</v>
       </c>
     </row>
     <row r="6" ht="200" customHeight="1" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A6" t="s">
-        <v>325</v>
+        <v>311</v>
       </c>
       <c r="B6" t="s">
-        <v>326</v>
+        <v>312</v>
       </c>
       <c r="C6" t="s">
-        <v>327</v>
+        <v>313</v>
       </c>
     </row>
     <row r="7" ht="200" customHeight="1" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A7" t="s">
-        <v>328</v>
+        <v>314</v>
       </c>
       <c r="B7" t="s">
-        <v>329</v>
+        <v>315</v>
       </c>
       <c r="C7" t="s">
-        <v>330</v>
+        <v>316</v>
       </c>
     </row>
     <row r="8" ht="200" customHeight="1" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A8" t="s">
-        <v>331</v>
+        <v>317</v>
       </c>
       <c r="B8" t="s">
-        <v>332</v>
+        <v>318</v>
       </c>
       <c r="C8" t="s">
-        <v>333</v>
+        <v>319</v>
       </c>
     </row>
     <row r="9" ht="200" customHeight="1" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A9" t="s">
-        <v>334</v>
+        <v>320</v>
       </c>
       <c r="B9" t="s">
-        <v>335</v>
+        <v>321</v>
       </c>
       <c r="C9" t="s">
-        <v>336</v>
+        <v>322</v>
       </c>
     </row>
     <row r="10" ht="200" customHeight="1" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A10" t="s">
-        <v>337</v>
+        <v>323</v>
       </c>
       <c r="B10" t="s">
-        <v>338</v>
+        <v>324</v>
       </c>
       <c r="C10" t="s">
-        <v>339</v>
+        <v>325</v>
       </c>
     </row>
     <row r="11" ht="200" customHeight="1" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A11" t="s">
-        <v>340</v>
+        <v>326</v>
       </c>
       <c r="B11" t="s">
-        <v>341</v>
+        <v>327</v>
       </c>
       <c r="C11" t="s">
-        <v>342</v>
+        <v>328</v>
       </c>
     </row>
     <row r="12" ht="200" customHeight="1" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A12" t="s">
-        <v>343</v>
+        <v>329</v>
       </c>
       <c r="B12" t="s">
-        <v>344</v>
+        <v>330</v>
       </c>
       <c r="C12" t="s">
-        <v>345</v>
+        <v>331</v>
       </c>
     </row>
     <row r="13" ht="200" customHeight="1" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A13" t="s">
-        <v>346</v>
+        <v>332</v>
       </c>
       <c r="B13" t="s">
-        <v>347</v>
+        <v>333</v>
       </c>
       <c r="C13" t="s">
-        <v>348</v>
+        <v>334</v>
       </c>
     </row>
     <row r="14" ht="200" customHeight="1" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A14" t="s">
-        <v>349</v>
+        <v>335</v>
       </c>
       <c r="B14" t="s">
-        <v>350</v>
+        <v>336</v>
       </c>
       <c r="C14" t="s">
-        <v>351</v>
+        <v>337</v>
       </c>
     </row>
     <row r="15" ht="200" customHeight="1" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A15" t="s">
-        <v>352</v>
+        <v>338</v>
       </c>
       <c r="B15" t="s">
-        <v>353</v>
+        <v>339</v>
       </c>
       <c r="C15" t="s">
-        <v>354</v>
+        <v>340</v>
       </c>
     </row>
     <row r="16" ht="200" customHeight="1" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A16" t="s">
-        <v>355</v>
+        <v>341</v>
       </c>
       <c r="B16" t="s">
-        <v>356</v>
+        <v>342</v>
       </c>
       <c r="C16" t="s">
-        <v>357</v>
+        <v>343</v>
       </c>
     </row>
     <row r="17" ht="200" customHeight="1" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A17" t="s">
-        <v>358</v>
+        <v>344</v>
       </c>
       <c r="B17" t="s">
-        <v>359</v>
+        <v>345</v>
       </c>
       <c r="C17" t="s">
-        <v>360</v>
+        <v>346</v>
       </c>
     </row>
     <row r="18" ht="200" customHeight="1" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A18" t="s">
-        <v>361</v>
+        <v>347</v>
       </c>
       <c r="B18" t="s">
-        <v>362</v>
+        <v>348</v>
       </c>
       <c r="C18" t="s">
-        <v>363</v>
+        <v>349</v>
       </c>
     </row>
     <row r="19" ht="200" customHeight="1" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A19" t="s">
-        <v>364</v>
+        <v>308</v>
       </c>
       <c r="B19" t="s">
-        <v>365</v>
+        <v>350</v>
       </c>
       <c r="C19" t="s">
-        <v>366</v>
+        <v>351</v>
       </c>
     </row>
     <row r="20" ht="200" customHeight="1" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A20" t="s">
-        <v>367</v>
+        <v>352</v>
       </c>
       <c r="B20" t="s">
-        <v>368</v>
+        <v>353</v>
       </c>
       <c r="C20" t="s">
-        <v>369</v>
+        <v>354</v>
       </c>
     </row>
     <row r="21" ht="200" customHeight="1" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A21" t="s">
-        <v>370</v>
+        <v>355</v>
       </c>
       <c r="B21" t="s">
-        <v>371</v>
+        <v>356</v>
       </c>
       <c r="C21" t="s">
-        <v>372</v>
+        <v>357</v>
       </c>
     </row>
     <row r="22" ht="200" customHeight="1" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A22" t="s">
-        <v>373</v>
+        <v>358</v>
       </c>
       <c r="B22" t="s">
-        <v>374</v>
+        <v>359</v>
       </c>
       <c r="C22" t="s">
-        <v>375</v>
+        <v>360</v>
       </c>
     </row>
     <row r="23" ht="200" customHeight="1" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A23" t="s">
-        <v>376</v>
+        <v>361</v>
       </c>
       <c r="B23" t="s">
-        <v>377</v>
+        <v>362</v>
       </c>
       <c r="C23" t="s">
-        <v>378</v>
+        <v>363</v>
       </c>
     </row>
     <row r="24" ht="200" customHeight="1" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A24" t="s">
-        <v>379</v>
+        <v>364</v>
       </c>
       <c r="B24" t="s">
-        <v>380</v>
+        <v>365</v>
       </c>
       <c r="C24" t="s">
-        <v>381</v>
+        <v>366</v>
       </c>
     </row>
     <row r="25" ht="200" customHeight="1" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A25" t="s">
-        <v>382</v>
+        <v>367</v>
       </c>
       <c r="B25" t="s">
-        <v>383</v>
+        <v>368</v>
       </c>
       <c r="C25" t="s">
-        <v>384</v>
+        <v>369</v>
       </c>
     </row>
     <row r="26" ht="200" customHeight="1" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A26" t="s">
-        <v>385</v>
+        <v>370</v>
       </c>
       <c r="B26" t="s">
-        <v>386</v>
+        <v>371</v>
       </c>
       <c r="C26" t="s">
-        <v>387</v>
+        <v>372</v>
       </c>
     </row>
     <row r="27" ht="200" customHeight="1" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A27" t="s">
-        <v>388</v>
+        <v>373</v>
       </c>
       <c r="B27" t="s">
-        <v>389</v>
+        <v>374</v>
       </c>
       <c r="C27" t="s">
-        <v>390</v>
+        <v>375</v>
       </c>
     </row>
     <row r="28" ht="200" customHeight="1" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A28" t="s">
-        <v>391</v>
+        <v>376</v>
       </c>
       <c r="B28" t="s">
-        <v>392</v>
+        <v>377</v>
       </c>
       <c r="C28" t="s">
-        <v>393</v>
+        <v>378</v>
       </c>
     </row>
     <row r="29" ht="200" customHeight="1" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A29" t="s">
-        <v>394</v>
+        <v>379</v>
       </c>
       <c r="B29" t="s">
-        <v>395</v>
+        <v>380</v>
       </c>
       <c r="C29" t="s">
-        <v>396</v>
+        <v>381</v>
       </c>
     </row>
     <row r="30" ht="200" customHeight="1" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A30" t="s">
-        <v>397</v>
+        <v>382</v>
       </c>
       <c r="B30" t="s">
-        <v>398</v>
+        <v>383</v>
       </c>
       <c r="C30" t="s">
-        <v>399</v>
+        <v>384</v>
       </c>
     </row>
     <row r="31" ht="200" customHeight="1" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A31" t="s">
-        <v>400</v>
+        <v>385</v>
       </c>
       <c r="B31" t="s">
-        <v>401</v>
+        <v>386</v>
       </c>
       <c r="C31" t="s">
-        <v>402</v>
+        <v>387</v>
       </c>
     </row>
     <row r="32" ht="200" customHeight="1" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A32" t="s">
-        <v>403</v>
+        <v>388</v>
       </c>
       <c r="B32" t="s">
-        <v>404</v>
+        <v>389</v>
       </c>
       <c r="C32" t="s">
-        <v>405</v>
+        <v>390</v>
       </c>
     </row>
     <row r="33" ht="200" customHeight="1" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A33" t="s">
-        <v>406</v>
+        <v>391</v>
       </c>
       <c r="B33" t="s">
-        <v>407</v>
+        <v>392</v>
       </c>
       <c r="C33" t="s">
-        <v>408</v>
+        <v>393</v>
       </c>
     </row>
     <row r="34" ht="200" customHeight="1" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A34" t="s">
+        <v>394</v>
+      </c>
+      <c r="B34" t="s">
+        <v>395</v>
+      </c>
+      <c r="C34" t="s">
+        <v>396</v>
+      </c>
+    </row>
+    <row r="35" ht="200" customHeight="1" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A35" t="s">
+        <v>397</v>
+      </c>
+      <c r="B35" t="s">
+        <v>398</v>
+      </c>
+      <c r="C35" t="s">
+        <v>399</v>
+      </c>
+    </row>
+    <row r="36" ht="200" customHeight="1" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A36" t="s">
+        <v>400</v>
+      </c>
+      <c r="B36" t="s">
+        <v>401</v>
+      </c>
+      <c r="C36" t="s">
+        <v>402</v>
+      </c>
+    </row>
+    <row r="37" ht="200" customHeight="1" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A37" t="s">
+        <v>403</v>
+      </c>
+      <c r="B37" t="s">
+        <v>404</v>
+      </c>
+      <c r="C37" t="s">
+        <v>405</v>
+      </c>
+    </row>
+    <row r="38" ht="200" customHeight="1" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A38" t="s">
+        <v>406</v>
+      </c>
+      <c r="B38" t="s">
+        <v>407</v>
+      </c>
+      <c r="C38" t="s">
+        <v>408</v>
+      </c>
+    </row>
+    <row r="39" ht="200" customHeight="1" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A39" t="s">
         <v>409</v>
       </c>
+      <c r="B39" t="s">
+        <v>410</v>
+      </c>
+      <c r="C39" t="s">
+        <v>411</v>
+      </c>
+    </row>
+    <row r="40" ht="200" customHeight="1" spans="3:3" x14ac:dyDescent="0.25">
+      <c r="C40" t="s">
+        <v>412</v>
+      </c>
+    </row>
+  </sheetData>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+  <pageSetup orientation="portrait" horizontalDpi="4294967295" verticalDpi="4294967295" scale="100" fitToWidth="1" fitToHeight="1"/>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet4.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+  <dimension ref="A1:E51"/>
+  <sheetFormatPr defaultRowHeight="15" outlineLevelRow="0" outlineLevelCol="0" x14ac:dyDescent="55"/>
+  <cols>
+    <col min="1" max="1" width="100" customWidth="1"/>
+    <col min="2" max="2" width="20" customWidth="1"/>
+    <col min="3" max="3" width="50" customWidth="1"/>
+    <col min="4" max="5" width="10" customWidth="1"/>
+  </cols>
+  <sheetData>
+    <row r="1" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A1" t="s">
+        <v>0</v>
+      </c>
+      <c r="B1" t="s">
+        <v>297</v>
+      </c>
+      <c r="C1" t="s">
+        <v>1</v>
+      </c>
+      <c r="D1" t="s">
+        <v>413</v>
+      </c>
+      <c r="E1" t="s">
+        <v>414</v>
+      </c>
+    </row>
+    <row r="2" ht="200" customHeight="1" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A2" t="s">
+        <v>415</v>
+      </c>
+      <c r="B2" t="s">
+        <v>416</v>
+      </c>
+      <c r="C2" t="s">
+        <v>417</v>
+      </c>
+      <c r="D2">
+        <v>20</v>
+      </c>
+      <c r="E2">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="3" ht="200" customHeight="1" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A3" t="s">
+        <v>418</v>
+      </c>
+      <c r="B3" t="s">
+        <v>419</v>
+      </c>
+      <c r="C3" t="s">
+        <v>420</v>
+      </c>
+      <c r="D3">
+        <v>3</v>
+      </c>
+      <c r="E3">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="4" ht="200" customHeight="1" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A4" t="s">
+        <v>99</v>
+      </c>
+      <c r="B4" t="s">
+        <v>419</v>
+      </c>
+      <c r="C4" t="s">
+        <v>421</v>
+      </c>
+      <c r="D4">
+        <v>11</v>
+      </c>
+      <c r="E4">
+        <v>14</v>
+      </c>
+    </row>
+    <row r="5" ht="200" customHeight="1" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A5" t="s">
+        <v>422</v>
+      </c>
+      <c r="B5" t="s">
+        <v>423</v>
+      </c>
+      <c r="C5" t="s">
+        <v>424</v>
+      </c>
+      <c r="D5">
+        <v>11</v>
+      </c>
+      <c r="E5">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="6" ht="200" customHeight="1" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A6" t="s">
+        <v>108</v>
+      </c>
+      <c r="B6" t="s">
+        <v>419</v>
+      </c>
+      <c r="C6" t="s">
+        <v>425</v>
+      </c>
+      <c r="D6">
+        <v>12</v>
+      </c>
+      <c r="E6">
+        <v>4</v>
+      </c>
+    </row>
+    <row r="7" ht="200" customHeight="1" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A7" t="s">
+        <v>426</v>
+      </c>
+      <c r="B7" t="s">
+        <v>419</v>
+      </c>
+      <c r="C7" t="s">
+        <v>427</v>
+      </c>
+      <c r="D7">
+        <v>28</v>
+      </c>
+      <c r="E7">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="8" ht="200" customHeight="1" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A8" t="s">
+        <v>81</v>
+      </c>
+      <c r="B8" t="s">
+        <v>419</v>
+      </c>
+      <c r="C8" t="s">
+        <v>428</v>
+      </c>
+      <c r="D8">
+        <v>3</v>
+      </c>
+      <c r="E8">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="9" ht="200" customHeight="1" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A9" t="s">
+        <v>429</v>
+      </c>
+      <c r="B9" t="s">
+        <v>423</v>
+      </c>
+      <c r="C9" t="s">
+        <v>430</v>
+      </c>
+      <c r="D9">
+        <v>0</v>
+      </c>
+      <c r="E9">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="10" ht="200" customHeight="1" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A10" t="s">
+        <v>431</v>
+      </c>
+      <c r="B10" t="s">
+        <v>416</v>
+      </c>
+      <c r="C10" t="s">
+        <v>432</v>
+      </c>
+      <c r="D10">
+        <v>6</v>
+      </c>
+      <c r="E10">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="11" ht="200" customHeight="1" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A11" t="s">
+        <v>433</v>
+      </c>
+      <c r="B11" t="s">
+        <v>416</v>
+      </c>
+      <c r="C11" t="s">
+        <v>434</v>
+      </c>
+      <c r="D11">
+        <v>17</v>
+      </c>
+      <c r="E11">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="12" ht="200" customHeight="1" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A12" t="s">
+        <v>435</v>
+      </c>
+      <c r="B12" t="s">
+        <v>423</v>
+      </c>
+      <c r="C12" t="s">
+        <v>436</v>
+      </c>
+      <c r="D12">
+        <v>2</v>
+      </c>
+      <c r="E12">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="13" ht="200" customHeight="1" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A13" t="s">
+        <v>87</v>
+      </c>
+      <c r="B13" t="s">
+        <v>419</v>
+      </c>
+      <c r="C13" t="s">
+        <v>437</v>
+      </c>
+      <c r="D13">
+        <v>10</v>
+      </c>
+      <c r="E13">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="14" ht="200" customHeight="1" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A14" t="s">
+        <v>438</v>
+      </c>
+      <c r="B14" t="s">
+        <v>439</v>
+      </c>
+      <c r="C14" t="s">
+        <v>440</v>
+      </c>
+      <c r="D14">
+        <v>2</v>
+      </c>
+      <c r="E14">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="15" ht="200" customHeight="1" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A15" t="s">
+        <v>441</v>
+      </c>
+      <c r="B15" t="s">
+        <v>442</v>
+      </c>
+      <c r="C15" t="s">
+        <v>443</v>
+      </c>
+      <c r="D15">
+        <v>38</v>
+      </c>
+      <c r="E15">
+        <v>3</v>
+      </c>
+    </row>
+    <row r="16" ht="200" customHeight="1" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A16" t="s">
+        <v>444</v>
+      </c>
+      <c r="B16" t="s">
+        <v>445</v>
+      </c>
+      <c r="C16" t="s">
+        <v>446</v>
+      </c>
+      <c r="D16">
+        <v>6</v>
+      </c>
+      <c r="E16">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="17" ht="200" customHeight="1" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A17" t="s">
+        <v>447</v>
+      </c>
+      <c r="B17" t="s">
+        <v>439</v>
+      </c>
+      <c r="C17" t="s">
+        <v>448</v>
+      </c>
+      <c r="D17">
+        <v>12</v>
+      </c>
+      <c r="E17">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="18" ht="200" customHeight="1" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A18" t="s">
+        <v>449</v>
+      </c>
+      <c r="B18" t="s">
+        <v>442</v>
+      </c>
+      <c r="C18" t="s">
+        <v>450</v>
+      </c>
+      <c r="D18">
+        <v>19</v>
+      </c>
+      <c r="E18">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="19" ht="200" customHeight="1" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A19" t="s">
+        <v>451</v>
+      </c>
+      <c r="B19" t="s">
+        <v>442</v>
+      </c>
+      <c r="C19" t="s">
+        <v>452</v>
+      </c>
+      <c r="D19">
+        <v>6</v>
+      </c>
+      <c r="E19">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="20" ht="200" customHeight="1" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A20" t="s">
+        <v>216</v>
+      </c>
+      <c r="B20" t="s">
+        <v>419</v>
+      </c>
+      <c r="C20" t="s">
+        <v>453</v>
+      </c>
+      <c r="D20">
+        <v>4</v>
+      </c>
+      <c r="E20">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="21" ht="200" customHeight="1" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A21" t="s">
+        <v>454</v>
+      </c>
+      <c r="B21" t="s">
+        <v>442</v>
+      </c>
+      <c r="C21" t="s">
+        <v>455</v>
+      </c>
+      <c r="D21">
+        <v>59</v>
+      </c>
+      <c r="E21">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="22" ht="200" customHeight="1" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A22" t="s">
+        <v>195</v>
+      </c>
+      <c r="B22" t="s">
+        <v>419</v>
+      </c>
+      <c r="C22" t="s">
+        <v>456</v>
+      </c>
+      <c r="D22">
+        <v>6</v>
+      </c>
+      <c r="E22">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="23" ht="200" customHeight="1" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A23" t="s">
+        <v>222</v>
+      </c>
+      <c r="B23" t="s">
+        <v>419</v>
+      </c>
+      <c r="C23" t="s">
+        <v>457</v>
+      </c>
+      <c r="D23">
+        <v>15</v>
+      </c>
+      <c r="E23">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="24" ht="200" customHeight="1" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A24" t="s">
+        <v>243</v>
+      </c>
+      <c r="B24" t="s">
+        <v>419</v>
+      </c>
+      <c r="C24" t="s">
+        <v>458</v>
+      </c>
+      <c r="D24">
+        <v>3</v>
+      </c>
+      <c r="E24">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="25" ht="200" customHeight="1" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A25" t="s">
+        <v>192</v>
+      </c>
+      <c r="B25" t="s">
+        <v>419</v>
+      </c>
+      <c r="C25" t="s">
+        <v>459</v>
+      </c>
+      <c r="D25">
+        <v>4</v>
+      </c>
+      <c r="E25">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="26" ht="200" customHeight="1" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A26" t="s">
+        <v>189</v>
+      </c>
+      <c r="B26" t="s">
+        <v>419</v>
+      </c>
+      <c r="C26" t="s">
+        <v>460</v>
+      </c>
+      <c r="D26">
+        <v>26</v>
+      </c>
+      <c r="E26">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="27" ht="200" customHeight="1" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A27" t="s">
+        <v>249</v>
+      </c>
+      <c r="B27" t="s">
+        <v>419</v>
+      </c>
+      <c r="C27" t="s">
+        <v>461</v>
+      </c>
+      <c r="D27">
+        <v>5</v>
+      </c>
+      <c r="E27">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="28" ht="200" customHeight="1" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A28" t="s">
+        <v>462</v>
+      </c>
+      <c r="B28" t="s">
+        <v>445</v>
+      </c>
+      <c r="C28" t="s">
+        <v>463</v>
+      </c>
+      <c r="D28">
+        <v>26</v>
+      </c>
+      <c r="E28">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="29" ht="200" customHeight="1" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A29" t="s">
+        <v>464</v>
+      </c>
+      <c r="B29" t="s">
+        <v>445</v>
+      </c>
+      <c r="C29" t="s">
+        <v>465</v>
+      </c>
+      <c r="D29">
+        <v>3</v>
+      </c>
+      <c r="E29">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="30" ht="200" customHeight="1" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A30" t="s">
+        <v>285</v>
+      </c>
+      <c r="B30" t="s">
+        <v>419</v>
+      </c>
+      <c r="C30" t="s">
+        <v>466</v>
+      </c>
+      <c r="D30">
+        <v>5</v>
+      </c>
+      <c r="E30">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="31" ht="200" customHeight="1" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A31" t="s">
+        <v>467</v>
+      </c>
+      <c r="B31" t="s">
+        <v>442</v>
+      </c>
+      <c r="C31" t="s">
+        <v>468</v>
+      </c>
+      <c r="D31">
+        <v>22</v>
+      </c>
+      <c r="E31">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="32" ht="200" customHeight="1" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A32" t="s">
+        <v>469</v>
+      </c>
+      <c r="B32" t="s">
+        <v>419</v>
+      </c>
+      <c r="C32" t="s">
+        <v>470</v>
+      </c>
+      <c r="D32">
+        <v>14</v>
+      </c>
+      <c r="E32">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="33" ht="200" customHeight="1" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A33" t="s">
+        <v>471</v>
+      </c>
+      <c r="B33" t="s">
+        <v>442</v>
+      </c>
+      <c r="C33" t="s">
+        <v>472</v>
+      </c>
+      <c r="D33">
+        <v>1</v>
+      </c>
+      <c r="E33">
+        <v>16</v>
+      </c>
+    </row>
+    <row r="34" ht="200" customHeight="1" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A34" t="s">
+        <v>473</v>
+      </c>
       <c r="B34" t="s">
-        <v>410</v>
+        <v>474</v>
       </c>
       <c r="C34" t="s">
-        <v>411</v>
+        <v>475</v>
+      </c>
+      <c r="D34">
+        <v>3</v>
+      </c>
+      <c r="E34">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="35" ht="200" customHeight="1" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A35" t="s">
+        <v>476</v>
+      </c>
+      <c r="B35" t="s">
+        <v>445</v>
+      </c>
+      <c r="C35" t="s">
+        <v>477</v>
+      </c>
+      <c r="D35">
+        <v>9</v>
+      </c>
+      <c r="E35">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="36" ht="200" customHeight="1" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A36" t="s">
+        <v>478</v>
+      </c>
+      <c r="B36" t="s">
+        <v>445</v>
+      </c>
+      <c r="C36" t="s">
+        <v>479</v>
+      </c>
+      <c r="D36">
+        <v>0</v>
+      </c>
+      <c r="E36">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="37" ht="200" customHeight="1" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A37" t="s">
+        <v>480</v>
+      </c>
+      <c r="B37" t="s">
+        <v>419</v>
+      </c>
+      <c r="C37" t="s">
+        <v>481</v>
+      </c>
+      <c r="D37">
+        <v>25</v>
+      </c>
+      <c r="E37">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="38" ht="200" customHeight="1" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A38" t="s">
+        <v>482</v>
+      </c>
+      <c r="B38" t="s">
+        <v>419</v>
+      </c>
+      <c r="C38" t="s">
+        <v>483</v>
+      </c>
+      <c r="D38">
+        <v>19</v>
+      </c>
+      <c r="E38">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="39" ht="200" customHeight="1" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A39" t="s">
+        <v>484</v>
+      </c>
+      <c r="B39" t="s">
+        <v>442</v>
+      </c>
+      <c r="C39" t="s">
+        <v>485</v>
+      </c>
+      <c r="D39">
+        <v>36</v>
+      </c>
+      <c r="E39">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="40" ht="200" customHeight="1" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A40" t="s">
+        <v>486</v>
+      </c>
+      <c r="B40" t="s">
+        <v>442</v>
+      </c>
+      <c r="C40" t="s">
+        <v>487</v>
+      </c>
+      <c r="D40">
+        <v>4</v>
+      </c>
+      <c r="E40">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="41" ht="200" customHeight="1" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A41" t="s">
+        <v>488</v>
+      </c>
+      <c r="B41" t="s">
+        <v>419</v>
+      </c>
+      <c r="C41" t="s">
+        <v>489</v>
+      </c>
+      <c r="D41">
+        <v>17</v>
+      </c>
+      <c r="E41">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="42" ht="200" customHeight="1" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A42" t="s">
+        <v>490</v>
+      </c>
+      <c r="B42" t="s">
+        <v>445</v>
+      </c>
+      <c r="C42" t="s">
+        <v>491</v>
+      </c>
+      <c r="D42">
+        <v>1</v>
+      </c>
+      <c r="E42">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="43" ht="200" customHeight="1" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A43" t="s">
+        <v>492</v>
+      </c>
+      <c r="B43" t="s">
+        <v>419</v>
+      </c>
+      <c r="C43" t="s">
+        <v>493</v>
+      </c>
+      <c r="D43">
+        <v>5</v>
+      </c>
+      <c r="E43">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="44" ht="200" customHeight="1" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A44" t="s">
+        <v>494</v>
+      </c>
+      <c r="B44" t="s">
+        <v>442</v>
+      </c>
+      <c r="C44" t="s">
+        <v>495</v>
+      </c>
+      <c r="D44">
+        <v>48</v>
+      </c>
+      <c r="E44">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="45" ht="200" customHeight="1" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A45" t="s">
+        <v>496</v>
+      </c>
+      <c r="B45" t="s">
+        <v>419</v>
+      </c>
+      <c r="C45" t="s">
+        <v>497</v>
+      </c>
+      <c r="D45">
+        <v>5</v>
+      </c>
+      <c r="E45">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="46" ht="200" customHeight="1" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A46" t="s">
+        <v>498</v>
+      </c>
+      <c r="B46" t="s">
+        <v>419</v>
+      </c>
+      <c r="C46" t="s">
+        <v>499</v>
+      </c>
+      <c r="D46">
+        <v>30</v>
+      </c>
+      <c r="E46">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="47" ht="200" customHeight="1" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A47" t="s">
+        <v>500</v>
+      </c>
+      <c r="B47" t="s">
+        <v>419</v>
+      </c>
+      <c r="C47" t="s">
+        <v>501</v>
+      </c>
+      <c r="D47">
+        <v>3</v>
+      </c>
+      <c r="E47">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="48" ht="200" customHeight="1" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A48" t="s">
+        <v>502</v>
+      </c>
+      <c r="B48" t="s">
+        <v>419</v>
+      </c>
+      <c r="C48" t="s">
+        <v>503</v>
+      </c>
+      <c r="D48">
+        <v>2</v>
+      </c>
+      <c r="E48">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="49" ht="200" customHeight="1" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A49" t="s">
+        <v>504</v>
+      </c>
+      <c r="B49" t="s">
+        <v>419</v>
+      </c>
+      <c r="C49" t="s">
+        <v>505</v>
+      </c>
+      <c r="D49">
+        <v>1</v>
+      </c>
+      <c r="E49">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="50" ht="200" customHeight="1" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A50" t="s">
+        <v>506</v>
+      </c>
+      <c r="B50" t="s">
+        <v>419</v>
+      </c>
+      <c r="C50" t="s">
+        <v>507</v>
+      </c>
+      <c r="D50">
+        <v>2</v>
+      </c>
+      <c r="E50">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="51" ht="200" customHeight="1" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A51" t="s">
+        <v>508</v>
+      </c>
+      <c r="B51" t="s">
+        <v>445</v>
+      </c>
+      <c r="C51" t="s">
+        <v>509</v>
+      </c>
+      <c r="D51">
+        <v>63</v>
+      </c>
+      <c r="E51">
+        <v>1</v>
       </c>
     </row>
   </sheetData>

</xml_diff>